<commit_message>
Major update on the refining some codes
</commit_message>
<xml_diff>
--- a/Sample Output/highlight.xlsx
+++ b/Sample Output/highlight.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="78">
   <si>
     <t>Original Currency</t>
   </si>
@@ -91,148 +91,163 @@
     <t>Million</t>
   </si>
   <si>
-    <t>2014</t>
-  </si>
-  <si>
-    <t>01733</t>
-  </si>
-  <si>
-    <t>WINSWAY</t>
-  </si>
-  <si>
-    <t>00809</t>
-  </si>
-  <si>
-    <t>GLOBAL BIO-CHEM</t>
-  </si>
-  <si>
     <t>2015</t>
   </si>
   <si>
-    <t>00094</t>
-  </si>
-  <si>
-    <t>GREENHEART GP</t>
-  </si>
-  <si>
-    <t>08163</t>
-  </si>
-  <si>
-    <t>MERDEKA FIN</t>
-  </si>
-  <si>
-    <t>08186</t>
-  </si>
-  <si>
-    <t>IR RESOURCES</t>
-  </si>
-  <si>
-    <t>00300</t>
-  </si>
-  <si>
-    <t>KUNMING MACHINE</t>
-  </si>
-  <si>
-    <t>01198</t>
-  </si>
-  <si>
-    <t>ROYALE FURN</t>
-  </si>
-  <si>
-    <t>00187</t>
-  </si>
-  <si>
-    <t>JINGCHENG MAC</t>
-  </si>
-  <si>
-    <t>00515</t>
-  </si>
-  <si>
-    <t>TC ORI LIGHT</t>
-  </si>
-  <si>
-    <t>00103</t>
-  </si>
-  <si>
-    <t>SHOUGANG CENT</t>
-  </si>
-  <si>
-    <t>00697</t>
-  </si>
-  <si>
-    <t>SHOUGANG INT'L</t>
-  </si>
-  <si>
-    <t>02889</t>
-  </si>
-  <si>
-    <t>NRI HOLDINGS</t>
-  </si>
-  <si>
-    <t>01132</t>
-  </si>
-  <si>
-    <t>ORANGE SKY G H</t>
-  </si>
-  <si>
-    <t>08228</t>
-  </si>
-  <si>
-    <t>NATIONAL ARTS</t>
-  </si>
-  <si>
-    <t>02178</t>
-  </si>
-  <si>
-    <t>PETRO-KING</t>
-  </si>
-  <si>
-    <t>00629</t>
-  </si>
-  <si>
-    <t>YUE DA MINING</t>
-  </si>
-  <si>
-    <t>01080</t>
-  </si>
-  <si>
-    <t>SHENGLI PIPE</t>
-  </si>
-  <si>
-    <t>00760</t>
-  </si>
-  <si>
-    <t>TALENT PPT GP</t>
-  </si>
-  <si>
-    <t>08272</t>
-  </si>
-  <si>
-    <t>C FOOD&amp;BEV; GP</t>
-  </si>
-  <si>
-    <t>00351</t>
-  </si>
-  <si>
-    <t>ASIA ENERGY LOG</t>
-  </si>
-  <si>
-    <t>00402</t>
-  </si>
-  <si>
-    <t>PEACEMAP HOLD</t>
-  </si>
-  <si>
-    <t>08045</t>
-  </si>
-  <si>
-    <t>NANDASOFT</t>
-  </si>
-  <si>
-    <t>00381</t>
-  </si>
-  <si>
-    <t>KIU HUNG INT'L</t>
+    <t>03818</t>
+  </si>
+  <si>
+    <t>CHINA DONGXIANG</t>
+  </si>
+  <si>
+    <t>00511</t>
+  </si>
+  <si>
+    <t>TVB</t>
+  </si>
+  <si>
+    <t>00054</t>
+  </si>
+  <si>
+    <t>HOPEWELL HOLD</t>
+  </si>
+  <si>
+    <t>00006</t>
+  </si>
+  <si>
+    <t>POWER ASSETS</t>
+  </si>
+  <si>
+    <t>01038</t>
+  </si>
+  <si>
+    <t>CKI HOLDINGS</t>
+  </si>
+  <si>
+    <t>00586</t>
+  </si>
+  <si>
+    <t>CONCH VENTURE</t>
+  </si>
+  <si>
+    <t>2016</t>
+  </si>
+  <si>
+    <t>00336</t>
+  </si>
+  <si>
+    <t>HUABAO INTL</t>
+  </si>
+  <si>
+    <t>01999</t>
+  </si>
+  <si>
+    <t>MAN WAH HLDGS</t>
+  </si>
+  <si>
+    <t>00273</t>
+  </si>
+  <si>
+    <t>MASON FIN</t>
+  </si>
+  <si>
+    <t>01066</t>
+  </si>
+  <si>
+    <t>WEIGAO GROUP</t>
+  </si>
+  <si>
+    <t>00460</t>
+  </si>
+  <si>
+    <t>SIHUAN PHARM</t>
+  </si>
+  <si>
+    <t>00587</t>
+  </si>
+  <si>
+    <t>HUA HAN HEALTH</t>
+  </si>
+  <si>
+    <t>02010</t>
+  </si>
+  <si>
+    <t>REAL NUTRI</t>
+  </si>
+  <si>
+    <t>00083</t>
+  </si>
+  <si>
+    <t>SINO LAND</t>
+  </si>
+  <si>
+    <t>01113</t>
+  </si>
+  <si>
+    <t>CK PROPERTY</t>
+  </si>
+  <si>
+    <t>00014</t>
+  </si>
+  <si>
+    <t>HYSAN DEV</t>
+  </si>
+  <si>
+    <t>00075</t>
+  </si>
+  <si>
+    <t>Y.T. REALTY</t>
+  </si>
+  <si>
+    <t>00225</t>
+  </si>
+  <si>
+    <t>POKFULAM</t>
+  </si>
+  <si>
+    <t>00251</t>
+  </si>
+  <si>
+    <t>SEA HOLDINGS</t>
+  </si>
+  <si>
+    <t>00064</t>
+  </si>
+  <si>
+    <t>GET NICE</t>
+  </si>
+  <si>
+    <t>00622</t>
+  </si>
+  <si>
+    <t>ENERCHINA HOLD</t>
+  </si>
+  <si>
+    <t>2013</t>
+  </si>
+  <si>
+    <t>01149</t>
+  </si>
+  <si>
+    <t>ANXIN-CHINA</t>
+  </si>
+  <si>
+    <t>00071</t>
+  </si>
+  <si>
+    <t>MIRAMAR HOTEL</t>
+  </si>
+  <si>
+    <t>00678</t>
+  </si>
+  <si>
+    <t>GENTING HK</t>
+  </si>
+  <si>
+    <t>00270</t>
+  </si>
+  <si>
+    <t>GUANGDONG INV</t>
   </si>
 </sst>
 </file>
@@ -570,7 +585,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X23"/>
+  <dimension ref="A1:Z23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
@@ -580,10 +595,10 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="25" width="15.7109375" customWidth="1"/>
+    <col min="2" max="27" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:26">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -656,8 +671,14 @@
       <c r="X1" t="s">
         <v>23</v>
       </c>
+      <c r="Y1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:26">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -730,8 +751,14 @@
       <c r="X2" t="s">
         <v>24</v>
       </c>
+      <c r="Y2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:26">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -742,37 +769,37 @@
         <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H3" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="I3" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="J3" t="s">
         <v>25</v>
       </c>
       <c r="K3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="L3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="M3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="N3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="O3" t="s">
         <v>25</v>
@@ -784,28 +811,34 @@
         <v>25</v>
       </c>
       <c r="R3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="S3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="T3" t="s">
         <v>25</v>
       </c>
       <c r="U3" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="V3" t="s">
         <v>25</v>
       </c>
       <c r="W3" t="s">
-        <v>30</v>
+        <v>69</v>
       </c>
       <c r="X3" t="s">
-        <v>30</v>
+        <v>25</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:26">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -816,16 +849,16 @@
         <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H4" t="s">
         <v>39</v>
@@ -873,13 +906,19 @@
         <v>67</v>
       </c>
       <c r="W4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="X4" t="s">
-        <v>71</v>
+        <v>72</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:26">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -890,16 +929,16 @@
         <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H5" t="s">
         <v>40</v>
@@ -947,1342 +986,1456 @@
         <v>68</v>
       </c>
       <c r="W5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="X5" t="s">
-        <v>72</v>
+        <v>73</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:26">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>1.35</v>
+        <v>55.48</v>
       </c>
       <c r="C6" s="1">
-        <v>-13.9</v>
+        <v>54.9</v>
       </c>
       <c r="D6" s="1">
-        <v>19.23</v>
+        <v>58.55</v>
       </c>
       <c r="E6" s="1">
-        <v>14.24</v>
+        <v>99.39</v>
       </c>
       <c r="F6" s="1">
-        <v>27.8</v>
+        <v>100</v>
       </c>
       <c r="G6" s="1">
-        <v>15.03</v>
+        <v>37.99</v>
       </c>
       <c r="H6" s="1">
-        <v>16.67</v>
+        <v>68.87</v>
       </c>
       <c r="I6" s="1">
-        <v>5.69</v>
+        <v>39.52</v>
       </c>
       <c r="J6" s="1">
-        <v>7.42</v>
+        <v>100</v>
       </c>
       <c r="K6" s="1">
-        <v>1.29</v>
+        <v>59.4</v>
       </c>
       <c r="L6" s="1">
-        <v>-15.61</v>
+        <v>70.35</v>
       </c>
       <c r="M6" s="1">
-        <v>-220.02</v>
+        <v>68.67</v>
       </c>
       <c r="N6" s="1">
-        <v>57.08</v>
+        <v>65.36</v>
       </c>
       <c r="O6" s="1">
-        <v>100</v>
+        <v>26.56</v>
       </c>
       <c r="P6" s="1">
         <v>100</v>
       </c>
       <c r="Q6" s="1">
-        <v>-7.61</v>
+        <v>87.93</v>
       </c>
       <c r="R6" s="1">
-        <v>1.95</v>
+        <v>97.58</v>
       </c>
       <c r="S6" s="1">
-        <v>21.06</v>
+        <v>62.8</v>
       </c>
       <c r="T6" s="1">
-        <v>0.59</v>
+        <v>100</v>
       </c>
       <c r="U6" s="1">
-        <v>11.07</v>
+        <v>100</v>
       </c>
       <c r="V6" s="1">
-        <v>21.76</v>
+        <v>100</v>
       </c>
       <c r="W6" s="1">
-        <v>13.26</v>
+        <v>78.53</v>
       </c>
       <c r="X6" s="1">
-        <v>35.68</v>
+        <v>63.25</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>100</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>66.99</v>
       </c>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:26">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>-5.3</v>
+        <v>69.1</v>
       </c>
       <c r="C7" s="1">
-        <v>-36.48</v>
+        <v>26.53</v>
       </c>
       <c r="D7" s="1">
-        <v>-80.41</v>
+        <v>188.42</v>
       </c>
       <c r="E7" s="1">
-        <v>-65.23</v>
+        <v>114.98</v>
       </c>
       <c r="F7" s="1">
-        <v>-3.55</v>
+        <v>158.68</v>
       </c>
       <c r="G7" s="1">
-        <v>-19.1</v>
+        <v>40.31</v>
       </c>
       <c r="H7" s="1">
-        <v>-2.99</v>
+        <v>50.44</v>
       </c>
       <c r="I7" s="1">
-        <v>-26.43</v>
+        <v>22.62</v>
       </c>
       <c r="J7" s="1">
-        <v>-10.59</v>
+        <v>37.93</v>
       </c>
       <c r="K7" s="1">
-        <v>-13.51</v>
+        <v>28.66</v>
       </c>
       <c r="L7" s="1">
-        <v>-27.58</v>
+        <v>92.46</v>
       </c>
       <c r="M7" s="1">
-        <v>-1761.3</v>
+        <v>63</v>
       </c>
       <c r="N7" s="1">
-        <v>-0.61</v>
+        <v>42.94</v>
       </c>
       <c r="O7" s="1">
-        <v>-254.61</v>
+        <v>44.81</v>
       </c>
       <c r="P7" s="1">
-        <v>-41.7</v>
+        <v>44.47</v>
       </c>
       <c r="Q7" s="1">
-        <v>-13.41</v>
+        <v>94.49</v>
       </c>
       <c r="R7" s="1">
-        <v>-7.73</v>
+        <v>139.81</v>
       </c>
       <c r="S7" s="1">
-        <v>-22.2</v>
+        <v>79.1</v>
       </c>
       <c r="T7" s="1">
-        <v>-235.44</v>
+        <v>178.28</v>
       </c>
       <c r="U7" s="1">
-        <v>-201.64</v>
+        <v>95.19</v>
       </c>
       <c r="V7" s="1">
-        <v>-47.06</v>
+        <v>826.32</v>
       </c>
       <c r="W7" s="1">
-        <v>-11.02</v>
+        <v>73.87</v>
       </c>
       <c r="X7" s="1">
-        <v>-21.02</v>
+        <v>49.42</v>
+      </c>
+      <c r="Y7" s="1">
+        <v>318.64</v>
+      </c>
+      <c r="Z7" s="1">
+        <v>67.3</v>
       </c>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:26">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>-48.93</v>
+        <v>54.66</v>
       </c>
       <c r="C8" s="1">
-        <v>-52.68</v>
+        <v>29.88</v>
       </c>
       <c r="D8" s="1">
-        <v>-73.88</v>
+        <v>152.01</v>
       </c>
       <c r="E8" s="1">
-        <v>-95.09</v>
+        <v>591.13</v>
       </c>
       <c r="F8" s="1">
-        <v>-90.16</v>
+        <v>183.16</v>
       </c>
       <c r="G8" s="1">
-        <v>-25.29</v>
+        <v>94.5</v>
       </c>
       <c r="H8" s="1">
-        <v>-14.77</v>
+        <v>36.92</v>
       </c>
       <c r="I8" s="1">
-        <v>-19.3</v>
+        <v>18.11</v>
       </c>
       <c r="J8" s="1">
-        <v>-15.85</v>
+        <v>209.94</v>
       </c>
       <c r="K8" s="1">
-        <v>-25.46</v>
+        <v>18.8</v>
       </c>
       <c r="L8" s="1">
-        <v>-46.05</v>
+        <v>65.12</v>
       </c>
       <c r="M8" s="1">
-        <v>-3160.23</v>
+        <v>35.63</v>
       </c>
       <c r="N8" s="1">
-        <v>-14.13</v>
+        <v>19.55</v>
       </c>
       <c r="O8" s="1">
-        <v>-646.32</v>
+        <v>42.91</v>
       </c>
       <c r="P8" s="1">
-        <v>-59.96</v>
+        <v>29.58</v>
       </c>
       <c r="Q8" s="1">
-        <v>-166.19</v>
+        <v>84.64</v>
       </c>
       <c r="R8" s="1">
-        <v>-15.46</v>
+        <v>244.34</v>
       </c>
       <c r="S8" s="1">
-        <v>-31.46</v>
+        <v>130.17</v>
       </c>
       <c r="T8" s="1">
-        <v>-385.88</v>
+        <v>195.98</v>
       </c>
       <c r="U8" s="1">
-        <v>-503.85</v>
+        <v>79.78</v>
       </c>
       <c r="V8" s="1">
-        <v>-107.01</v>
+        <v>657.49</v>
       </c>
       <c r="W8" s="1">
-        <v>-31.26</v>
+        <v>55.01</v>
       </c>
       <c r="X8" s="1">
-        <v>-40.15</v>
+        <v>41.69</v>
+      </c>
+      <c r="Y8" s="1">
+        <v>306.21</v>
+      </c>
+      <c r="Z8" s="1">
+        <v>42.58</v>
       </c>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:26">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>-1.15</v>
+        <v>0</v>
       </c>
       <c r="C9" s="2">
-        <v>-2.99</v>
+        <v>183.51</v>
       </c>
       <c r="D9" s="2">
-        <v>-13</v>
+        <v>36.6</v>
       </c>
       <c r="E9" s="2">
-        <v>-5.19</v>
+        <v>5.7</v>
       </c>
       <c r="F9" s="2">
-        <v>-0.05</v>
+        <v>13.32</v>
       </c>
       <c r="G9" s="2">
-        <v>-3.35</v>
+        <v>21.56</v>
       </c>
       <c r="H9" s="2">
-        <v>-0.83</v>
+        <v>157.79</v>
       </c>
       <c r="I9" s="2">
-        <v>-20.85</v>
+        <v>138.53</v>
       </c>
       <c r="J9" s="2">
-        <v>-8.19</v>
+        <v>23.19</v>
       </c>
       <c r="K9" s="2">
-        <v>-4.07</v>
+        <v>35.7</v>
       </c>
       <c r="L9" s="2">
-        <v>-4.21</v>
+        <v>18302.44</v>
       </c>
       <c r="M9" s="2">
-        <v>-1.51</v>
+        <v>30.12</v>
       </c>
       <c r="N9" s="2">
-        <v>-0.18</v>
+        <v>16.32</v>
       </c>
       <c r="O9" s="2">
-        <v>-0.72</v>
+        <v>40.95</v>
       </c>
       <c r="P9" s="2">
-        <v>-7.2</v>
+        <v>18.55</v>
       </c>
       <c r="Q9" s="2">
-        <v>-1.12</v>
+        <v>15.89</v>
       </c>
       <c r="R9" s="2">
-        <v>-2.6</v>
+        <v>245.38</v>
       </c>
       <c r="S9" s="2">
-        <v>-0.57</v>
+        <v>51.02</v>
       </c>
       <c r="T9" s="2">
-        <v>-1.69</v>
+        <v>10.37</v>
       </c>
       <c r="U9" s="2">
-        <v>-0.65</v>
+        <v>272.95</v>
       </c>
       <c r="V9" s="2">
-        <v>-1.75</v>
+        <v>57.92</v>
       </c>
       <c r="W9" s="2">
-        <v>-1.56</v>
+        <v>56.06</v>
       </c>
       <c r="X9" s="2">
-        <v>-3.2</v>
+        <v>47.5</v>
+      </c>
+      <c r="Y9" s="2">
+        <v>85.21</v>
+      </c>
+      <c r="Z9" s="2">
+        <v>45.39</v>
       </c>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:26">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>1.1</v>
+        <v>6.04</v>
       </c>
       <c r="C10" s="2">
-        <v>0.44</v>
+        <v>8.8</v>
       </c>
       <c r="D10" s="2">
-        <v>0.43</v>
+        <v>5.64</v>
       </c>
       <c r="E10" s="2">
-        <v>1.41</v>
+        <v>32.35</v>
       </c>
       <c r="F10" s="2">
-        <v>0.14</v>
+        <v>2.52</v>
       </c>
       <c r="G10" s="2">
-        <v>1.13</v>
+        <v>2.88</v>
       </c>
       <c r="H10" s="2">
-        <v>0.89</v>
+        <v>6.64</v>
       </c>
       <c r="I10" s="2">
-        <v>1.11</v>
+        <v>3.05</v>
       </c>
       <c r="J10" s="2">
-        <v>1.08</v>
+        <v>10.62</v>
       </c>
       <c r="K10" s="2">
-        <v>1.04</v>
+        <v>3.78</v>
       </c>
       <c r="L10" s="2">
-        <v>0.29</v>
+        <v>5.83</v>
       </c>
       <c r="M10" s="2">
-        <v>0.17</v>
+        <v>11.15</v>
       </c>
       <c r="N10" s="2">
-        <v>0.83</v>
+        <v>4.21</v>
       </c>
       <c r="O10" s="2">
-        <v>0.13</v>
+        <v>3.99</v>
       </c>
       <c r="P10" s="2">
-        <v>1.22</v>
+        <v>5.77</v>
       </c>
       <c r="Q10" s="2">
-        <v>0.96</v>
+        <v>2.34</v>
       </c>
       <c r="R10" s="2">
-        <v>1.31</v>
+        <v>2.31</v>
       </c>
       <c r="S10" s="2">
-        <v>0.7</v>
+        <v>2.01</v>
       </c>
       <c r="T10" s="2">
-        <v>0.17</v>
+        <v>2.28</v>
       </c>
       <c r="U10" s="2">
-        <v>0.1</v>
+        <v>4.82</v>
       </c>
       <c r="V10" s="2">
-        <v>0.54</v>
+        <v>40.37</v>
       </c>
       <c r="W10" s="2">
-        <v>0.66</v>
+        <v>8.01</v>
       </c>
       <c r="X10" s="2">
-        <v>0.81</v>
+        <v>2.74</v>
+      </c>
+      <c r="Y10" s="2">
+        <v>6.82</v>
+      </c>
+      <c r="Z10" s="2">
+        <v>2.85</v>
       </c>
     </row>
-    <row r="11" spans="1:24">
+    <row r="11" spans="1:26">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>0.19</v>
+        <v>1.24</v>
       </c>
       <c r="C11" s="2">
-        <v>0.08</v>
+        <v>3.91</v>
       </c>
       <c r="D11" s="2">
-        <v>0.21</v>
+        <v>2.95</v>
       </c>
       <c r="E11" s="2">
-        <v>0.13</v>
+        <v>32.16</v>
       </c>
       <c r="F11" s="2">
-        <v>0.03</v>
+        <v>2.15</v>
       </c>
       <c r="G11" s="2">
-        <v>0.08</v>
+        <v>1.84</v>
       </c>
       <c r="H11" s="2">
-        <v>0.25</v>
+        <v>3.65</v>
       </c>
       <c r="I11" s="2">
-        <v>0.23</v>
+        <v>1.55</v>
       </c>
       <c r="J11" s="2">
-        <v>0.37</v>
+        <v>1.33</v>
       </c>
       <c r="K11" s="2">
-        <v>0.15</v>
+        <v>1.85</v>
       </c>
       <c r="L11" s="2">
-        <v>0.07</v>
+        <v>2.44</v>
       </c>
       <c r="M11" s="2">
-        <v>0.04</v>
+        <v>9.64</v>
       </c>
       <c r="N11" s="2">
-        <v>0.3</v>
+        <v>3.03</v>
       </c>
       <c r="O11" s="2">
-        <v>0.02</v>
+        <v>1.53</v>
       </c>
       <c r="P11" s="2">
-        <v>0.2</v>
+        <v>1.25</v>
       </c>
       <c r="Q11" s="2">
-        <v>0.36</v>
+        <v>1.92</v>
       </c>
       <c r="R11" s="2">
-        <v>0.39</v>
+        <v>2.27</v>
       </c>
       <c r="S11" s="2">
-        <v>0.05</v>
+        <v>1.39</v>
       </c>
       <c r="T11" s="2">
-        <v>0.01</v>
+        <v>1.81</v>
       </c>
       <c r="U11" s="2">
-        <v>0.02</v>
+        <v>1.08</v>
       </c>
       <c r="V11" s="2">
-        <v>0.11</v>
+        <v>9.93</v>
       </c>
       <c r="W11" s="2">
-        <v>0.1</v>
+        <v>7.25</v>
       </c>
       <c r="X11" s="2">
-        <v>0.05</v>
+        <v>2.41</v>
+      </c>
+      <c r="Y11" s="2">
+        <v>3.29</v>
+      </c>
+      <c r="Z11" s="2">
+        <v>1.61</v>
       </c>
     </row>
-    <row r="12" spans="1:24">
+    <row r="12" spans="1:26">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="2">
-        <v>300.38</v>
+        <v>11437.33</v>
       </c>
       <c r="C12" s="2">
-        <v>822.31</v>
+        <v>7680.43</v>
       </c>
       <c r="D12" s="2">
-        <v>580.49</v>
+        <v>45530</v>
       </c>
       <c r="E12" s="2">
-        <v>15.68</v>
+        <v>123597</v>
       </c>
       <c r="F12" s="2">
-        <v>178.85</v>
+        <v>102571</v>
       </c>
       <c r="G12" s="2">
-        <v>1067.01</v>
+        <v>19510.14</v>
       </c>
       <c r="H12" s="2">
-        <v>1105.81</v>
+        <v>10187.24</v>
       </c>
       <c r="I12" s="2">
-        <v>855.2</v>
+        <v>4712.34</v>
       </c>
       <c r="J12" s="2">
-        <v>373.21</v>
+        <v>3026.46</v>
       </c>
       <c r="K12" s="2">
-        <v>1395.87</v>
+        <v>12789.81</v>
       </c>
       <c r="L12" s="2">
-        <v>1336.31</v>
+        <v>13314.77</v>
       </c>
       <c r="M12" s="2">
-        <v>277.16</v>
+        <v>8559.67</v>
       </c>
       <c r="N12" s="2">
-        <v>1579.84</v>
+        <v>6690.94</v>
       </c>
       <c r="O12" s="2">
-        <v>1072.47</v>
+        <v>118558</v>
       </c>
       <c r="P12" s="2">
-        <v>1751.63</v>
+        <v>263096</v>
       </c>
       <c r="Q12" s="2">
-        <v>635.46</v>
+        <v>68172</v>
       </c>
       <c r="R12" s="2">
-        <v>1999.28</v>
+        <v>6616.02</v>
       </c>
       <c r="S12" s="2">
-        <v>164.47</v>
+        <v>4385.59</v>
       </c>
       <c r="T12" s="2">
-        <v>-86.28</v>
+        <v>13074.4</v>
       </c>
       <c r="U12" s="2">
-        <v>390.23</v>
+        <v>4839.36</v>
       </c>
       <c r="V12" s="2">
-        <v>552.67</v>
+        <v>5041.96</v>
       </c>
       <c r="W12" s="2">
-        <v>263.36</v>
+        <v>4102.28</v>
       </c>
       <c r="X12" s="2">
-        <v>389.6</v>
+        <v>14183.04</v>
+      </c>
+      <c r="Y12" s="2">
+        <v>42483.32</v>
+      </c>
+      <c r="Z12" s="2">
+        <v>31472</v>
       </c>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13" spans="1:26">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="1">
-        <v>34.57</v>
+        <v>4.3</v>
       </c>
       <c r="C13" s="1">
-        <v>63.18</v>
+        <v>2.58</v>
       </c>
       <c r="D13" s="1">
-        <v>49.73</v>
+        <v>8.43</v>
       </c>
       <c r="E13" s="1">
-        <v>89.72</v>
+        <v>6.95</v>
       </c>
       <c r="F13" s="1">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G13" s="1">
-        <v>18.94</v>
+        <v>2.86</v>
       </c>
       <c r="H13" s="1">
-        <v>23.77</v>
+        <v>0.16</v>
       </c>
       <c r="I13" s="1">
-        <v>9.91</v>
+        <v>4.43</v>
       </c>
       <c r="J13" s="1">
-        <v>20.23</v>
+        <v>7.17</v>
       </c>
       <c r="K13" s="1">
-        <v>37.19</v>
+        <v>7.54</v>
       </c>
       <c r="L13" s="1">
-        <v>38.74</v>
+        <v>0.07</v>
       </c>
       <c r="M13" s="1">
-        <v>58.24</v>
+        <v>0.31</v>
       </c>
       <c r="N13" s="1">
-        <v>28.17</v>
+        <v>7.38</v>
       </c>
       <c r="O13" s="1">
-        <v>29.01</v>
+        <v>4.26</v>
       </c>
       <c r="P13" s="1">
-        <v>23.7</v>
+        <v>16.4</v>
       </c>
       <c r="Q13" s="1">
-        <v>17.25</v>
+        <v>6.17</v>
       </c>
       <c r="R13" s="1">
-        <v>31.92</v>
+        <v>1.19</v>
       </c>
       <c r="S13" s="1">
-        <v>61.32</v>
+        <v>1.54</v>
       </c>
       <c r="T13" s="1">
-        <v>103.07</v>
+        <v>23.53</v>
       </c>
       <c r="U13" s="1">
-        <v>65.66</v>
+        <v>7.19</v>
       </c>
       <c r="V13" s="1">
-        <v>44.4</v>
+        <v>1.83</v>
       </c>
       <c r="W13" s="1">
-        <v>20.6</v>
+        <v>1.94</v>
       </c>
       <c r="X13" s="1">
-        <v>36.82</v>
+        <v>8.39</v>
+      </c>
+      <c r="Y13" s="1">
+        <v>8.16</v>
+      </c>
+      <c r="Z13" s="1">
+        <v>13.99</v>
       </c>
     </row>
-    <row r="14" spans="1:24">
+    <row r="14" spans="1:26">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="1">
-        <v>1183.92</v>
+        <v>4.77</v>
       </c>
       <c r="C14" s="1">
-        <v>1056.9</v>
+        <v>3.06</v>
       </c>
       <c r="D14" s="1">
-        <v>123.18</v>
+        <v>10.23</v>
       </c>
       <c r="E14" s="1">
-        <v>6394.05</v>
+        <v>7.61</v>
       </c>
       <c r="F14" s="1">
-        <v>0</v>
+        <v>16.75</v>
       </c>
       <c r="G14" s="1">
-        <v>59.56</v>
+        <v>3.26</v>
       </c>
       <c r="H14" s="1">
-        <v>44.2</v>
+        <v>0.18</v>
       </c>
       <c r="I14" s="1">
-        <v>28.88</v>
+        <v>5.31</v>
       </c>
       <c r="J14" s="1">
-        <v>61.85</v>
+        <v>10.45</v>
       </c>
       <c r="K14" s="1">
-        <v>80.1</v>
+        <v>9.56</v>
       </c>
       <c r="L14" s="1">
-        <v>616.37</v>
+        <v>0.07</v>
       </c>
       <c r="M14" s="1">
-        <v>952.94</v>
+        <v>0.37</v>
       </c>
       <c r="N14" s="1">
-        <v>51.09</v>
+        <v>8.82</v>
       </c>
       <c r="O14" s="1">
-        <v>49.66</v>
+        <v>5.09</v>
       </c>
       <c r="P14" s="1">
-        <v>42.79</v>
+        <v>23.18</v>
       </c>
       <c r="Q14" s="1">
-        <v>35.85</v>
+        <v>7.13</v>
       </c>
       <c r="R14" s="1">
-        <v>66</v>
+        <v>1.23</v>
       </c>
       <c r="S14" s="1">
-        <v>1309.12</v>
+        <v>1.6</v>
       </c>
       <c r="T14" s="1">
-        <v>-410.58</v>
+        <v>34.34</v>
       </c>
       <c r="U14" s="1">
-        <v>386.53</v>
+        <v>8.99</v>
       </c>
       <c r="V14" s="1">
-        <v>149.76</v>
+        <v>2.01</v>
       </c>
       <c r="W14" s="1">
-        <v>123.47</v>
+        <v>2.13</v>
       </c>
       <c r="X14" s="1">
-        <v>76.3</v>
+        <v>10.03</v>
+      </c>
+      <c r="Y14" s="1">
+        <v>9.73</v>
+      </c>
+      <c r="Z14" s="1">
+        <v>24.06</v>
       </c>
     </row>
-    <row r="15" spans="1:24">
+    <row r="15" spans="1:26">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="2">
-        <v>16209.91</v>
+        <v>13133.84</v>
       </c>
       <c r="C15" s="2">
-        <v>16270.57</v>
+        <v>9834.97</v>
       </c>
       <c r="D15" s="2">
-        <v>1712.82</v>
+        <v>54955.5</v>
       </c>
       <c r="E15" s="2">
-        <v>630.13</v>
+        <v>135816</v>
       </c>
       <c r="F15" s="2">
-        <v>314.62</v>
+        <v>129086</v>
       </c>
       <c r="G15" s="2">
-        <v>3366.76</v>
+        <v>21423.95</v>
       </c>
       <c r="H15" s="2">
-        <v>2143.33</v>
+        <v>11243.54</v>
       </c>
       <c r="I15" s="2">
-        <v>2751.22</v>
+        <v>5870.42</v>
       </c>
       <c r="J15" s="2">
-        <v>1115.49</v>
+        <v>3504.02</v>
       </c>
       <c r="K15" s="2">
-        <v>3308.13</v>
+        <v>15353.61</v>
       </c>
       <c r="L15" s="2">
-        <v>23575.02</v>
+        <v>14186.39</v>
       </c>
       <c r="M15" s="2">
-        <v>5488.21</v>
+        <v>7990.07</v>
       </c>
       <c r="N15" s="2">
-        <v>2898.05</v>
+        <v>7540.83</v>
       </c>
       <c r="O15" s="2">
-        <v>1703.85</v>
+        <v>139366</v>
       </c>
       <c r="P15" s="2">
-        <v>3005.63</v>
+        <v>276358</v>
       </c>
       <c r="Q15" s="2">
-        <v>1566.18</v>
+        <v>78905.5</v>
       </c>
       <c r="R15" s="2">
-        <v>4370.64</v>
+        <v>6593.88</v>
       </c>
       <c r="S15" s="2">
-        <v>3702.27</v>
+        <v>4480.78</v>
       </c>
       <c r="T15" s="2">
-        <v>420.25</v>
+        <v>18513.64</v>
       </c>
       <c r="U15" s="2">
-        <v>2300</v>
+        <v>5793.91</v>
       </c>
       <c r="V15" s="2">
-        <v>1958.95</v>
+        <v>5040.54</v>
       </c>
       <c r="W15" s="2">
-        <v>1671.56</v>
+        <v>4292.75</v>
       </c>
       <c r="X15" s="2">
-        <v>634.61</v>
+        <v>17104.8</v>
+      </c>
+      <c r="Y15" s="2">
+        <v>40377.25</v>
+      </c>
+      <c r="Z15" s="2">
+        <v>50862.5</v>
       </c>
     </row>
-    <row r="16" spans="1:24">
+    <row r="16" spans="1:26">
       <c r="A16" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="2">
-        <v>3189.66</v>
+        <v>11944.58</v>
       </c>
       <c r="C16" s="2">
-        <v>3176.4</v>
+        <v>8270.26</v>
       </c>
       <c r="D16" s="2">
-        <v>701.87</v>
+        <v>47848.5</v>
       </c>
       <c r="E16" s="2">
-        <v>43.58</v>
+        <v>123342.5</v>
       </c>
       <c r="F16" s="2">
-        <v>182.65</v>
+        <v>106152.5</v>
       </c>
       <c r="G16" s="2">
-        <v>1272.21</v>
+        <v>19229.91</v>
       </c>
       <c r="H16" s="2">
-        <v>1211.72</v>
+        <v>9967.13</v>
       </c>
       <c r="I16" s="2">
-        <v>1556.84</v>
+        <v>4581.34</v>
       </c>
       <c r="J16" s="2">
-        <v>393.58</v>
+        <v>3310.41</v>
       </c>
       <c r="K16" s="2">
-        <v>1628.88</v>
+        <v>12399.85</v>
       </c>
       <c r="L16" s="2">
-        <v>2231.67</v>
+        <v>12358.65</v>
       </c>
       <c r="M16" s="2">
-        <v>979.21</v>
+        <v>7108.14</v>
       </c>
       <c r="N16" s="2">
-        <v>1686.93</v>
+        <v>6138.41</v>
       </c>
       <c r="O16" s="2">
-        <v>890.95</v>
+        <v>115987.5</v>
       </c>
       <c r="P16" s="2">
-        <v>2010.25</v>
+        <v>193439.5</v>
       </c>
       <c r="Q16" s="2">
-        <v>922.17</v>
+        <v>70748.5</v>
       </c>
       <c r="R16" s="2">
-        <v>2430.36</v>
+        <v>6327.29</v>
       </c>
       <c r="S16" s="2">
-        <v>203.33</v>
+        <v>4324.45</v>
       </c>
       <c r="T16" s="2">
-        <v>2.65</v>
+        <v>13071.56</v>
       </c>
       <c r="U16" s="2">
-        <v>671.47</v>
+        <v>4352.28</v>
       </c>
       <c r="V16" s="2">
-        <v>711.42</v>
+        <v>4730.41</v>
       </c>
       <c r="W16" s="2">
-        <v>407.92</v>
+        <v>3757.47</v>
       </c>
       <c r="X16" s="2">
-        <v>347.11</v>
+        <v>13811.17</v>
+      </c>
+      <c r="Y16" s="2">
+        <v>34002.22</v>
+      </c>
+      <c r="Z16" s="2">
+        <v>36465.5</v>
       </c>
     </row>
-    <row r="17" spans="1:24">
+    <row r="17" spans="1:26">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="1">
-        <v>-22.78</v>
+        <v>7.34</v>
       </c>
       <c r="C17" s="1">
-        <v>-20.72</v>
+        <v>13.54</v>
       </c>
       <c r="D17" s="1">
-        <v>-25.51</v>
+        <v>5.16</v>
       </c>
       <c r="E17" s="1">
-        <v>-19.83</v>
+        <v>5.69</v>
       </c>
       <c r="F17" s="1">
-        <v>-11.15</v>
+        <v>8.65</v>
       </c>
       <c r="G17" s="1">
-        <v>-7</v>
+        <v>10.89</v>
       </c>
       <c r="H17" s="1">
-        <v>-4.55</v>
+        <v>12.9</v>
       </c>
       <c r="I17" s="1">
-        <v>-9.06</v>
+        <v>22.61</v>
       </c>
       <c r="J17" s="1">
-        <v>-10.03</v>
+        <v>10.19</v>
       </c>
       <c r="K17" s="1">
-        <v>-11.4</v>
+        <v>8.7</v>
       </c>
       <c r="L17" s="1">
-        <v>-14.21</v>
+        <v>17.45</v>
       </c>
       <c r="M17" s="1">
-        <v>-26.74</v>
+        <v>8.12</v>
       </c>
       <c r="N17" s="1">
-        <v>-6.23</v>
+        <v>6.38</v>
       </c>
       <c r="O17" s="1">
-        <v>-8.74</v>
+        <v>6.72</v>
       </c>
       <c r="P17" s="1">
-        <v>-14.08</v>
+        <v>6.19</v>
       </c>
       <c r="Q17" s="1">
-        <v>-17.16</v>
+        <v>3.68</v>
       </c>
       <c r="R17" s="1">
-        <v>-8.3</v>
+        <v>8.1</v>
       </c>
       <c r="S17" s="1">
-        <v>-3.11</v>
+        <v>3.85</v>
       </c>
       <c r="T17" s="1">
-        <v>-42.95</v>
+        <v>7.76</v>
       </c>
       <c r="U17" s="1">
-        <v>-8.04</v>
+        <v>8</v>
       </c>
       <c r="V17" s="1">
-        <v>-18.23</v>
+        <v>14.15</v>
       </c>
       <c r="W17" s="1">
-        <v>-11.51</v>
+        <v>8.61</v>
       </c>
       <c r="X17" s="1">
-        <v>-14.13</v>
+        <v>7.92</v>
+      </c>
+      <c r="Y17" s="1">
+        <v>40.71</v>
+      </c>
+      <c r="Z17" s="1">
+        <v>7.68</v>
       </c>
     </row>
-    <row r="18" spans="1:24">
+    <row r="18" spans="1:26">
       <c r="A18" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="2">
-        <v>5.08</v>
+        <v>1.1</v>
       </c>
       <c r="C18" s="2">
-        <v>5.12</v>
+        <v>1.19</v>
       </c>
       <c r="D18" s="2">
-        <v>2.44</v>
+        <v>1.15</v>
       </c>
       <c r="E18" s="2">
-        <v>14.46</v>
+        <v>1.1</v>
       </c>
       <c r="F18" s="2">
-        <v>1.72</v>
+        <v>1.22</v>
       </c>
       <c r="G18" s="2">
-        <v>2.65</v>
+        <v>1.11</v>
       </c>
       <c r="H18" s="2">
-        <v>1.77</v>
+        <v>1.13</v>
       </c>
       <c r="I18" s="2">
-        <v>1.77</v>
+        <v>1.28</v>
       </c>
       <c r="J18" s="2">
-        <v>2.83</v>
+        <v>1.06</v>
       </c>
       <c r="K18" s="2">
-        <v>2.03</v>
+        <v>1.24</v>
       </c>
       <c r="L18" s="2">
-        <v>10.56</v>
+        <v>1.15</v>
       </c>
       <c r="M18" s="2">
-        <v>5.6</v>
+        <v>1.12</v>
       </c>
       <c r="N18" s="2">
-        <v>1.72</v>
+        <v>1.23</v>
       </c>
       <c r="O18" s="2">
-        <v>1.91</v>
+        <v>1.2</v>
       </c>
       <c r="P18" s="2">
-        <v>1.5</v>
+        <v>1.43</v>
       </c>
       <c r="Q18" s="2">
-        <v>1.7</v>
+        <v>1.12</v>
       </c>
       <c r="R18" s="2">
-        <v>1.8</v>
+        <v>1.04</v>
       </c>
       <c r="S18" s="2">
-        <v>18.21</v>
+        <v>1.04</v>
       </c>
       <c r="T18" s="2">
-        <v>158.55</v>
+        <v>1.42</v>
       </c>
       <c r="U18" s="2">
-        <v>3.43</v>
+        <v>1.33</v>
       </c>
       <c r="V18" s="2">
-        <v>2.75</v>
+        <v>1.07</v>
       </c>
       <c r="W18" s="2">
-        <v>4.1</v>
+        <v>1.14</v>
       </c>
       <c r="X18" s="2">
-        <v>1.83</v>
+        <v>1.24</v>
+      </c>
+      <c r="Y18" s="2">
+        <v>1.19</v>
+      </c>
+      <c r="Z18" s="2">
+        <v>1.39</v>
       </c>
     </row>
-    <row r="19" spans="1:24">
+    <row r="19" spans="1:26">
       <c r="A19" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="1">
-        <v>6.13</v>
+        <v>5.57</v>
       </c>
       <c r="C19" s="1">
-        <v>38.72</v>
+        <v>4.27</v>
       </c>
       <c r="D19" s="1">
-        <v>50.06</v>
+        <v>11.16</v>
       </c>
       <c r="E19" s="1">
-        <v>187.01</v>
+        <v>7.21</v>
       </c>
       <c r="F19" s="1">
-        <v>0.68</v>
+        <v>16.69</v>
       </c>
       <c r="G19" s="1">
-        <v>3.54</v>
+        <v>4.89</v>
       </c>
       <c r="H19" s="1">
-        <v>0.24</v>
+        <v>7.34</v>
       </c>
       <c r="I19" s="1">
-        <v>4.23</v>
+        <v>6.55</v>
       </c>
       <c r="J19" s="1">
-        <v>3.01</v>
+        <v>4.09</v>
       </c>
       <c r="K19" s="1">
-        <v>3.13</v>
+        <v>3.09</v>
       </c>
       <c r="L19" s="1">
-        <v>41.4</v>
+        <v>18.52</v>
       </c>
       <c r="M19" s="1">
-        <v>2639.57</v>
+        <v>5.75</v>
       </c>
       <c r="N19" s="1">
-        <v>0.07</v>
+        <v>3.37</v>
       </c>
       <c r="O19" s="1">
-        <v>42.56</v>
+        <v>3.62</v>
       </c>
       <c r="P19" s="1">
-        <v>8.78</v>
+        <v>3.93</v>
       </c>
       <c r="Q19" s="1">
-        <v>3.91</v>
+        <v>3.88</v>
       </c>
       <c r="R19" s="1">
-        <v>1.15</v>
+        <v>11.81</v>
       </c>
       <c r="S19" s="1">
-        <v>12.57</v>
+        <v>3.15</v>
       </c>
       <c r="T19" s="1">
-        <v>16031.53</v>
+        <v>19.58</v>
       </c>
       <c r="U19" s="1">
-        <v>55.5</v>
+        <v>10.14</v>
       </c>
       <c r="V19" s="1">
-        <v>23.63</v>
+        <v>124.56</v>
       </c>
       <c r="W19" s="1">
-        <v>5.2</v>
+        <v>7.26</v>
       </c>
       <c r="X19" s="1">
-        <v>5.43</v>
+        <v>4.85</v>
+      </c>
+      <c r="Y19" s="1">
+        <v>154.03</v>
+      </c>
+      <c r="Z19" s="1">
+        <v>7.21</v>
       </c>
     </row>
-    <row r="20" spans="1:24">
+    <row r="20" spans="1:26">
       <c r="A20" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="2">
-        <v>1.31</v>
+        <v>10.54</v>
       </c>
       <c r="C20" s="2">
-        <v>0.77</v>
+        <v>29.06</v>
       </c>
       <c r="D20" s="2">
-        <v>1.48</v>
+        <v>2.83</v>
       </c>
       <c r="E20" s="2">
-        <v>1.28</v>
+        <v>10.09</v>
       </c>
       <c r="F20" s="2">
-        <v>-0.05</v>
+        <v>6.72</v>
       </c>
       <c r="G20" s="2">
-        <v>1.24</v>
+        <v>28.66</v>
       </c>
       <c r="H20" s="2">
-        <v>0.94</v>
+        <v>307.3</v>
       </c>
       <c r="I20" s="2">
-        <v>1.91</v>
+        <v>55.38</v>
       </c>
       <c r="J20" s="2">
-        <v>1.71</v>
+        <v>8.98</v>
       </c>
       <c r="K20" s="2">
-        <v>1.04</v>
+        <v>5.27</v>
       </c>
       <c r="L20" s="2">
-        <v>0.19</v>
+        <v>1200.01</v>
       </c>
       <c r="M20" s="2">
-        <v>0.3</v>
+        <v>94.76</v>
       </c>
       <c r="N20" s="2">
-        <v>1.65</v>
+        <v>2.04</v>
       </c>
       <c r="O20" s="2">
-        <v>0.84</v>
+        <v>8.02</v>
       </c>
       <c r="P20" s="2">
-        <v>1.54</v>
+        <v>2.66</v>
       </c>
       <c r="Q20" s="2">
-        <v>1.57</v>
+        <v>4.18</v>
       </c>
       <c r="R20" s="2">
-        <v>1.43</v>
+        <v>18.7</v>
       </c>
       <c r="S20" s="2">
-        <v>0.13</v>
+        <v>11.14</v>
       </c>
       <c r="T20" s="2">
-        <v>0.82</v>
+        <v>2.2</v>
       </c>
       <c r="U20" s="2">
-        <v>0.49</v>
+        <v>2.95</v>
       </c>
       <c r="V20" s="2">
-        <v>1.82</v>
+        <v>11.55</v>
       </c>
       <c r="W20" s="2">
-        <v>0.79</v>
+        <v>8.67</v>
       </c>
       <c r="X20" s="2">
-        <v>1.26</v>
+        <v>3.27</v>
+      </c>
+      <c r="Y20" s="2">
+        <v>21.31</v>
+      </c>
+      <c r="Z20" s="2">
+        <v>6.04</v>
       </c>
     </row>
-    <row r="21" spans="1:24">
+    <row r="21" spans="1:26">
       <c r="A21" t="s">
         <v>20</v>
       </c>
       <c r="B21" s="2">
-        <v>-0.06</v>
+        <v>9.26</v>
       </c>
       <c r="C21" s="2">
-        <v>-0.33</v>
+        <v>8.12</v>
       </c>
       <c r="D21" s="2">
-        <v>-1.42</v>
+        <v>7.37</v>
       </c>
       <c r="E21" s="2">
-        <v>-1.37</v>
+        <v>19.05</v>
       </c>
       <c r="F21" s="2">
-        <v>-1.62</v>
+        <v>16.77</v>
       </c>
       <c r="G21" s="2">
-        <v>-2.91</v>
+        <v>12.98</v>
       </c>
       <c r="H21" s="2">
-        <v>-4.29</v>
+        <v>6.35</v>
       </c>
       <c r="I21" s="2">
-        <v>-1.81</v>
+        <v>16.87</v>
       </c>
       <c r="J21" s="2">
-        <v>-2.34</v>
+        <v>12.06</v>
       </c>
       <c r="K21" s="2">
-        <v>-0.97</v>
+        <v>6.71</v>
       </c>
       <c r="L21" s="2">
-        <v>-0.54</v>
+        <v>8.03</v>
       </c>
       <c r="M21" s="2">
-        <v>-0.55</v>
+        <v>7.52</v>
       </c>
       <c r="N21" s="2">
-        <v>-7.95</v>
+        <v>2.76</v>
       </c>
       <c r="O21" s="2">
-        <v>-4.68</v>
+        <v>8.17</v>
       </c>
       <c r="P21" s="2">
-        <v>-2.15</v>
+        <v>10.48</v>
       </c>
       <c r="Q21" s="2">
-        <v>-1.28</v>
+        <v>11.48</v>
       </c>
       <c r="R21" s="2">
-        <v>-2.81</v>
+        <v>4.81</v>
       </c>
       <c r="S21" s="2">
-        <v>-6.4</v>
+        <v>7.55</v>
       </c>
       <c r="T21" s="2">
-        <v>-0.57</v>
+        <v>8.99</v>
       </c>
       <c r="U21" s="2">
-        <v>-7.12</v>
+        <v>3.18</v>
       </c>
       <c r="V21" s="2">
-        <v>-5.14</v>
+        <v>2.6</v>
       </c>
       <c r="W21" s="2">
-        <v>-0.84</v>
+        <v>3.19</v>
       </c>
       <c r="X21" s="2">
-        <v>-3.03</v>
+        <v>5.46</v>
+      </c>
+      <c r="Y21" s="2">
+        <v>9.13</v>
+      </c>
+      <c r="Z21" s="2">
+        <v>18.05</v>
       </c>
     </row>
-    <row r="22" spans="1:24">
+    <row r="22" spans="1:26">
       <c r="A22" t="s">
         <v>21</v>
       </c>
       <c r="B22" s="2">
-        <v>0.06</v>
+        <v>1.34</v>
       </c>
       <c r="C22" s="2">
-        <v>0.18</v>
+        <v>24.67</v>
       </c>
       <c r="D22" s="2">
-        <v>0.64</v>
+        <v>24.01</v>
       </c>
       <c r="E22" s="2">
-        <v>0.14</v>
+        <v>69.02</v>
       </c>
       <c r="F22" s="2">
-        <v>0.02</v>
+        <v>70.64</v>
       </c>
       <c r="G22" s="2">
-        <v>4.06</v>
+        <v>13.99</v>
       </c>
       <c r="H22" s="2">
-        <v>0.24</v>
+        <v>2.96</v>
       </c>
       <c r="I22" s="2">
-        <v>3.76</v>
+        <v>5.81</v>
       </c>
       <c r="J22" s="2">
-        <v>0.49</v>
+        <v>0.28</v>
       </c>
       <c r="K22" s="2">
-        <v>0.19</v>
+        <v>3.96</v>
       </c>
       <c r="L22" s="2">
-        <v>0.2</v>
+        <v>1.65</v>
       </c>
       <c r="M22" s="2">
-        <v>0.24</v>
+        <v>0.66</v>
       </c>
       <c r="N22" s="2">
-        <v>0.52</v>
+        <v>0.7</v>
       </c>
       <c r="O22" s="2">
-        <v>0.21</v>
+        <v>12.43</v>
       </c>
       <c r="P22" s="2">
-        <v>0.68</v>
+        <v>46.65</v>
       </c>
       <c r="Q22" s="2">
-        <v>0.31</v>
+        <v>31.86</v>
       </c>
       <c r="R22" s="2">
-        <v>0.31</v>
+        <v>3.21</v>
       </c>
       <c r="S22" s="2">
-        <v>0.19</v>
+        <v>11.82</v>
       </c>
       <c r="T22" s="2">
-        <v>0.19</v>
+        <v>18.98</v>
       </c>
       <c r="U22" s="2">
-        <v>0.09</v>
+        <v>0.22</v>
       </c>
       <c r="V22" s="2">
-        <v>0.22</v>
+        <v>0.26</v>
       </c>
       <c r="W22" s="2">
-        <v>0.32</v>
+        <v>0.39</v>
       </c>
       <c r="X22" s="2">
-        <v>0.06</v>
+        <v>12.81</v>
+      </c>
+      <c r="Y22" s="2">
+        <v>2.27</v>
+      </c>
+      <c r="Z22" s="2">
+        <v>11.25</v>
       </c>
     </row>
-    <row r="23" spans="1:24">
+    <row r="23" spans="1:26">
       <c r="A23" t="s">
         <v>22</v>
       </c>
       <c r="B23" s="2">
-        <v>0.08</v>
+        <v>1.69</v>
       </c>
       <c r="C23" s="2">
-        <v>0.18</v>
+        <v>26.75</v>
       </c>
       <c r="D23" s="2">
-        <v>0.73</v>
+        <v>27.25</v>
       </c>
       <c r="E23" s="2">
-        <v>0.1</v>
+        <v>77.4</v>
       </c>
       <c r="F23" s="2">
-        <v>0.02</v>
+        <v>69.25</v>
       </c>
       <c r="G23" s="2">
-        <v>3.06</v>
+        <v>15.24</v>
       </c>
       <c r="H23" s="2">
+        <v>2.88</v>
+      </c>
+      <c r="I23" s="2">
+        <v>5.77</v>
+      </c>
+      <c r="J23" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="K23" s="2">
+        <v>4.78</v>
+      </c>
+      <c r="L23" s="2">
+        <v>1.75</v>
+      </c>
+      <c r="M23" s="2">
+        <v>0.47</v>
+      </c>
+      <c r="N23" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="O23" s="2">
+        <v>13.62</v>
+      </c>
+      <c r="P23" s="2">
+        <v>54.8</v>
+      </c>
+      <c r="Q23" s="2">
+        <v>37.5</v>
+      </c>
+      <c r="R23" s="2">
+        <v>3.9</v>
+      </c>
+      <c r="S23" s="2">
+        <v>12.76</v>
+      </c>
+      <c r="T23" s="2">
+        <v>19.08</v>
+      </c>
+      <c r="U23" s="2">
+        <v>0.28</v>
+      </c>
+      <c r="V23" s="2">
         <v>0.33</v>
       </c>
-      <c r="I23" s="2">
-        <v>3.2</v>
-      </c>
-      <c r="J23" s="2">
-        <v>0.41</v>
-      </c>
-      <c r="K23" s="2">
-        <v>0.22</v>
-      </c>
-      <c r="L23" s="2">
-        <v>0.24</v>
-      </c>
-      <c r="M23" s="2">
-        <v>0.24</v>
-      </c>
-      <c r="N23" s="2">
-        <v>0.51</v>
-      </c>
-      <c r="O23" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="P23" s="2">
-        <v>0.57</v>
-      </c>
-      <c r="Q23" s="2">
-        <v>0.33</v>
-      </c>
-      <c r="R23" s="2">
-        <v>0.41</v>
-      </c>
-      <c r="S23" s="2">
-        <v>0.16</v>
-      </c>
-      <c r="T23" s="2">
-        <v>0.17</v>
-      </c>
-      <c r="U23" s="2">
-        <v>0.07</v>
-      </c>
-      <c r="V23" s="2">
-        <v>0.22</v>
-      </c>
       <c r="W23" s="2">
-        <v>0.4</v>
+        <v>0.39</v>
       </c>
       <c r="X23" s="2">
-        <v>0.06</v>
+        <v>13.68</v>
+      </c>
+      <c r="Y23" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="Z23" s="2">
+        <v>11.62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Major update on the refining some codes"
This reverts commit 5d588302a2f16858e3394a4ac10f54321eae69d1.
</commit_message>
<xml_diff>
--- a/Sample Output/highlight.xlsx
+++ b/Sample Output/highlight.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="73">
   <si>
     <t>Original Currency</t>
   </si>
@@ -91,163 +91,148 @@
     <t>Million</t>
   </si>
   <si>
+    <t>2014</t>
+  </si>
+  <si>
+    <t>01733</t>
+  </si>
+  <si>
+    <t>WINSWAY</t>
+  </si>
+  <si>
+    <t>00809</t>
+  </si>
+  <si>
+    <t>GLOBAL BIO-CHEM</t>
+  </si>
+  <si>
     <t>2015</t>
   </si>
   <si>
-    <t>03818</t>
-  </si>
-  <si>
-    <t>CHINA DONGXIANG</t>
-  </si>
-  <si>
-    <t>00511</t>
-  </si>
-  <si>
-    <t>TVB</t>
-  </si>
-  <si>
-    <t>00054</t>
-  </si>
-  <si>
-    <t>HOPEWELL HOLD</t>
-  </si>
-  <si>
-    <t>00006</t>
-  </si>
-  <si>
-    <t>POWER ASSETS</t>
-  </si>
-  <si>
-    <t>01038</t>
-  </si>
-  <si>
-    <t>CKI HOLDINGS</t>
-  </si>
-  <si>
-    <t>00586</t>
-  </si>
-  <si>
-    <t>CONCH VENTURE</t>
-  </si>
-  <si>
-    <t>2016</t>
-  </si>
-  <si>
-    <t>00336</t>
-  </si>
-  <si>
-    <t>HUABAO INTL</t>
-  </si>
-  <si>
-    <t>01999</t>
-  </si>
-  <si>
-    <t>MAN WAH HLDGS</t>
-  </si>
-  <si>
-    <t>00273</t>
-  </si>
-  <si>
-    <t>MASON FIN</t>
-  </si>
-  <si>
-    <t>01066</t>
-  </si>
-  <si>
-    <t>WEIGAO GROUP</t>
-  </si>
-  <si>
-    <t>00460</t>
-  </si>
-  <si>
-    <t>SIHUAN PHARM</t>
-  </si>
-  <si>
-    <t>00587</t>
-  </si>
-  <si>
-    <t>HUA HAN HEALTH</t>
-  </si>
-  <si>
-    <t>02010</t>
-  </si>
-  <si>
-    <t>REAL NUTRI</t>
-  </si>
-  <si>
-    <t>00083</t>
-  </si>
-  <si>
-    <t>SINO LAND</t>
-  </si>
-  <si>
-    <t>01113</t>
-  </si>
-  <si>
-    <t>CK PROPERTY</t>
-  </si>
-  <si>
-    <t>00014</t>
-  </si>
-  <si>
-    <t>HYSAN DEV</t>
-  </si>
-  <si>
-    <t>00075</t>
-  </si>
-  <si>
-    <t>Y.T. REALTY</t>
-  </si>
-  <si>
-    <t>00225</t>
-  </si>
-  <si>
-    <t>POKFULAM</t>
-  </si>
-  <si>
-    <t>00251</t>
-  </si>
-  <si>
-    <t>SEA HOLDINGS</t>
-  </si>
-  <si>
-    <t>00064</t>
-  </si>
-  <si>
-    <t>GET NICE</t>
-  </si>
-  <si>
-    <t>00622</t>
-  </si>
-  <si>
-    <t>ENERCHINA HOLD</t>
-  </si>
-  <si>
-    <t>2013</t>
-  </si>
-  <si>
-    <t>01149</t>
-  </si>
-  <si>
-    <t>ANXIN-CHINA</t>
-  </si>
-  <si>
-    <t>00071</t>
-  </si>
-  <si>
-    <t>MIRAMAR HOTEL</t>
-  </si>
-  <si>
-    <t>00678</t>
-  </si>
-  <si>
-    <t>GENTING HK</t>
-  </si>
-  <si>
-    <t>00270</t>
-  </si>
-  <si>
-    <t>GUANGDONG INV</t>
+    <t>00094</t>
+  </si>
+  <si>
+    <t>GREENHEART GP</t>
+  </si>
+  <si>
+    <t>08163</t>
+  </si>
+  <si>
+    <t>MERDEKA FIN</t>
+  </si>
+  <si>
+    <t>08186</t>
+  </si>
+  <si>
+    <t>IR RESOURCES</t>
+  </si>
+  <si>
+    <t>00300</t>
+  </si>
+  <si>
+    <t>KUNMING MACHINE</t>
+  </si>
+  <si>
+    <t>01198</t>
+  </si>
+  <si>
+    <t>ROYALE FURN</t>
+  </si>
+  <si>
+    <t>00187</t>
+  </si>
+  <si>
+    <t>JINGCHENG MAC</t>
+  </si>
+  <si>
+    <t>00515</t>
+  </si>
+  <si>
+    <t>TC ORI LIGHT</t>
+  </si>
+  <si>
+    <t>00103</t>
+  </si>
+  <si>
+    <t>SHOUGANG CENT</t>
+  </si>
+  <si>
+    <t>00697</t>
+  </si>
+  <si>
+    <t>SHOUGANG INT'L</t>
+  </si>
+  <si>
+    <t>02889</t>
+  </si>
+  <si>
+    <t>NRI HOLDINGS</t>
+  </si>
+  <si>
+    <t>01132</t>
+  </si>
+  <si>
+    <t>ORANGE SKY G H</t>
+  </si>
+  <si>
+    <t>08228</t>
+  </si>
+  <si>
+    <t>NATIONAL ARTS</t>
+  </si>
+  <si>
+    <t>02178</t>
+  </si>
+  <si>
+    <t>PETRO-KING</t>
+  </si>
+  <si>
+    <t>00629</t>
+  </si>
+  <si>
+    <t>YUE DA MINING</t>
+  </si>
+  <si>
+    <t>01080</t>
+  </si>
+  <si>
+    <t>SHENGLI PIPE</t>
+  </si>
+  <si>
+    <t>00760</t>
+  </si>
+  <si>
+    <t>TALENT PPT GP</t>
+  </si>
+  <si>
+    <t>08272</t>
+  </si>
+  <si>
+    <t>C FOOD&amp;BEV; GP</t>
+  </si>
+  <si>
+    <t>00351</t>
+  </si>
+  <si>
+    <t>ASIA ENERGY LOG</t>
+  </si>
+  <si>
+    <t>00402</t>
+  </si>
+  <si>
+    <t>PEACEMAP HOLD</t>
+  </si>
+  <si>
+    <t>08045</t>
+  </si>
+  <si>
+    <t>NANDASOFT</t>
+  </si>
+  <si>
+    <t>00381</t>
+  </si>
+  <si>
+    <t>KIU HUNG INT'L</t>
   </si>
 </sst>
 </file>
@@ -585,7 +570,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z23"/>
+  <dimension ref="A1:X23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
@@ -595,10 +580,10 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="27" width="15.7109375" customWidth="1"/>
+    <col min="2" max="25" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:24">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -671,14 +656,8 @@
       <c r="X1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>23</v>
-      </c>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:24">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -751,14 +730,8 @@
       <c r="X2" t="s">
         <v>24</v>
       </c>
-      <c r="Y2" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>24</v>
-      </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:24">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -769,37 +742,37 @@
         <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="H3" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="I3" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="J3" t="s">
         <v>25</v>
       </c>
       <c r="K3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="L3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="M3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="N3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="O3" t="s">
         <v>25</v>
@@ -811,34 +784,28 @@
         <v>25</v>
       </c>
       <c r="R3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="S3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="T3" t="s">
         <v>25</v>
       </c>
       <c r="U3" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="V3" t="s">
         <v>25</v>
       </c>
       <c r="W3" t="s">
-        <v>69</v>
+        <v>30</v>
       </c>
       <c r="X3" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:24">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -849,16 +816,16 @@
         <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H4" t="s">
         <v>39</v>
@@ -906,19 +873,13 @@
         <v>67</v>
       </c>
       <c r="W4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="X4" t="s">
-        <v>72</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>74</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:24">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -929,16 +890,16 @@
         <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H5" t="s">
         <v>40</v>
@@ -986,1456 +947,1342 @@
         <v>68</v>
       </c>
       <c r="W5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="X5" t="s">
-        <v>73</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>75</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:24">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>55.48</v>
+        <v>1.35</v>
       </c>
       <c r="C6" s="1">
-        <v>54.9</v>
+        <v>-13.9</v>
       </c>
       <c r="D6" s="1">
-        <v>58.55</v>
+        <v>19.23</v>
       </c>
       <c r="E6" s="1">
-        <v>99.39</v>
+        <v>14.24</v>
       </c>
       <c r="F6" s="1">
+        <v>27.8</v>
+      </c>
+      <c r="G6" s="1">
+        <v>15.03</v>
+      </c>
+      <c r="H6" s="1">
+        <v>16.67</v>
+      </c>
+      <c r="I6" s="1">
+        <v>5.69</v>
+      </c>
+      <c r="J6" s="1">
+        <v>7.42</v>
+      </c>
+      <c r="K6" s="1">
+        <v>1.29</v>
+      </c>
+      <c r="L6" s="1">
+        <v>-15.61</v>
+      </c>
+      <c r="M6" s="1">
+        <v>-220.02</v>
+      </c>
+      <c r="N6" s="1">
+        <v>57.08</v>
+      </c>
+      <c r="O6" s="1">
         <v>100</v>
-      </c>
-      <c r="G6" s="1">
-        <v>37.99</v>
-      </c>
-      <c r="H6" s="1">
-        <v>68.87</v>
-      </c>
-      <c r="I6" s="1">
-        <v>39.52</v>
-      </c>
-      <c r="J6" s="1">
-        <v>100</v>
-      </c>
-      <c r="K6" s="1">
-        <v>59.4</v>
-      </c>
-      <c r="L6" s="1">
-        <v>70.35</v>
-      </c>
-      <c r="M6" s="1">
-        <v>68.67</v>
-      </c>
-      <c r="N6" s="1">
-        <v>65.36</v>
-      </c>
-      <c r="O6" s="1">
-        <v>26.56</v>
       </c>
       <c r="P6" s="1">
         <v>100</v>
       </c>
       <c r="Q6" s="1">
-        <v>87.93</v>
+        <v>-7.61</v>
       </c>
       <c r="R6" s="1">
-        <v>97.58</v>
+        <v>1.95</v>
       </c>
       <c r="S6" s="1">
-        <v>62.8</v>
+        <v>21.06</v>
       </c>
       <c r="T6" s="1">
-        <v>100</v>
+        <v>0.59</v>
       </c>
       <c r="U6" s="1">
-        <v>100</v>
+        <v>11.07</v>
       </c>
       <c r="V6" s="1">
-        <v>100</v>
+        <v>21.76</v>
       </c>
       <c r="W6" s="1">
-        <v>78.53</v>
+        <v>13.26</v>
       </c>
       <c r="X6" s="1">
-        <v>63.25</v>
-      </c>
-      <c r="Y6" s="1">
-        <v>100</v>
-      </c>
-      <c r="Z6" s="1">
-        <v>66.99</v>
+        <v>35.68</v>
       </c>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:24">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>69.1</v>
+        <v>-5.3</v>
       </c>
       <c r="C7" s="1">
-        <v>26.53</v>
+        <v>-36.48</v>
       </c>
       <c r="D7" s="1">
-        <v>188.42</v>
+        <v>-80.41</v>
       </c>
       <c r="E7" s="1">
-        <v>114.98</v>
+        <v>-65.23</v>
       </c>
       <c r="F7" s="1">
-        <v>158.68</v>
+        <v>-3.55</v>
       </c>
       <c r="G7" s="1">
-        <v>40.31</v>
+        <v>-19.1</v>
       </c>
       <c r="H7" s="1">
-        <v>50.44</v>
+        <v>-2.99</v>
       </c>
       <c r="I7" s="1">
-        <v>22.62</v>
+        <v>-26.43</v>
       </c>
       <c r="J7" s="1">
-        <v>37.93</v>
+        <v>-10.59</v>
       </c>
       <c r="K7" s="1">
-        <v>28.66</v>
+        <v>-13.51</v>
       </c>
       <c r="L7" s="1">
-        <v>92.46</v>
+        <v>-27.58</v>
       </c>
       <c r="M7" s="1">
-        <v>63</v>
+        <v>-1761.3</v>
       </c>
       <c r="N7" s="1">
-        <v>42.94</v>
+        <v>-0.61</v>
       </c>
       <c r="O7" s="1">
-        <v>44.81</v>
+        <v>-254.61</v>
       </c>
       <c r="P7" s="1">
-        <v>44.47</v>
+        <v>-41.7</v>
       </c>
       <c r="Q7" s="1">
-        <v>94.49</v>
+        <v>-13.41</v>
       </c>
       <c r="R7" s="1">
-        <v>139.81</v>
+        <v>-7.73</v>
       </c>
       <c r="S7" s="1">
-        <v>79.1</v>
+        <v>-22.2</v>
       </c>
       <c r="T7" s="1">
-        <v>178.28</v>
+        <v>-235.44</v>
       </c>
       <c r="U7" s="1">
-        <v>95.19</v>
+        <v>-201.64</v>
       </c>
       <c r="V7" s="1">
-        <v>826.32</v>
+        <v>-47.06</v>
       </c>
       <c r="W7" s="1">
-        <v>73.87</v>
+        <v>-11.02</v>
       </c>
       <c r="X7" s="1">
-        <v>49.42</v>
-      </c>
-      <c r="Y7" s="1">
-        <v>318.64</v>
-      </c>
-      <c r="Z7" s="1">
-        <v>67.3</v>
+        <v>-21.02</v>
       </c>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:24">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>54.66</v>
+        <v>-48.93</v>
       </c>
       <c r="C8" s="1">
-        <v>29.88</v>
+        <v>-52.68</v>
       </c>
       <c r="D8" s="1">
-        <v>152.01</v>
+        <v>-73.88</v>
       </c>
       <c r="E8" s="1">
-        <v>591.13</v>
+        <v>-95.09</v>
       </c>
       <c r="F8" s="1">
-        <v>183.16</v>
+        <v>-90.16</v>
       </c>
       <c r="G8" s="1">
-        <v>94.5</v>
+        <v>-25.29</v>
       </c>
       <c r="H8" s="1">
-        <v>36.92</v>
+        <v>-14.77</v>
       </c>
       <c r="I8" s="1">
-        <v>18.11</v>
+        <v>-19.3</v>
       </c>
       <c r="J8" s="1">
-        <v>209.94</v>
+        <v>-15.85</v>
       </c>
       <c r="K8" s="1">
-        <v>18.8</v>
+        <v>-25.46</v>
       </c>
       <c r="L8" s="1">
-        <v>65.12</v>
+        <v>-46.05</v>
       </c>
       <c r="M8" s="1">
-        <v>35.63</v>
+        <v>-3160.23</v>
       </c>
       <c r="N8" s="1">
-        <v>19.55</v>
+        <v>-14.13</v>
       </c>
       <c r="O8" s="1">
-        <v>42.91</v>
+        <v>-646.32</v>
       </c>
       <c r="P8" s="1">
-        <v>29.58</v>
+        <v>-59.96</v>
       </c>
       <c r="Q8" s="1">
-        <v>84.64</v>
+        <v>-166.19</v>
       </c>
       <c r="R8" s="1">
-        <v>244.34</v>
+        <v>-15.46</v>
       </c>
       <c r="S8" s="1">
-        <v>130.17</v>
+        <v>-31.46</v>
       </c>
       <c r="T8" s="1">
-        <v>195.98</v>
+        <v>-385.88</v>
       </c>
       <c r="U8" s="1">
-        <v>79.78</v>
+        <v>-503.85</v>
       </c>
       <c r="V8" s="1">
-        <v>657.49</v>
+        <v>-107.01</v>
       </c>
       <c r="W8" s="1">
-        <v>55.01</v>
+        <v>-31.26</v>
       </c>
       <c r="X8" s="1">
-        <v>41.69</v>
-      </c>
-      <c r="Y8" s="1">
-        <v>306.21</v>
-      </c>
-      <c r="Z8" s="1">
-        <v>42.58</v>
+        <v>-40.15</v>
       </c>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:24">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>0</v>
+        <v>-1.15</v>
       </c>
       <c r="C9" s="2">
-        <v>183.51</v>
+        <v>-2.99</v>
       </c>
       <c r="D9" s="2">
-        <v>36.6</v>
+        <v>-13</v>
       </c>
       <c r="E9" s="2">
-        <v>5.7</v>
+        <v>-5.19</v>
       </c>
       <c r="F9" s="2">
-        <v>13.32</v>
+        <v>-0.05</v>
       </c>
       <c r="G9" s="2">
-        <v>21.56</v>
+        <v>-3.35</v>
       </c>
       <c r="H9" s="2">
-        <v>157.79</v>
+        <v>-0.83</v>
       </c>
       <c r="I9" s="2">
-        <v>138.53</v>
+        <v>-20.85</v>
       </c>
       <c r="J9" s="2">
-        <v>23.19</v>
+        <v>-8.19</v>
       </c>
       <c r="K9" s="2">
-        <v>35.7</v>
+        <v>-4.07</v>
       </c>
       <c r="L9" s="2">
-        <v>18302.44</v>
+        <v>-4.21</v>
       </c>
       <c r="M9" s="2">
-        <v>30.12</v>
+        <v>-1.51</v>
       </c>
       <c r="N9" s="2">
-        <v>16.32</v>
+        <v>-0.18</v>
       </c>
       <c r="O9" s="2">
-        <v>40.95</v>
+        <v>-0.72</v>
       </c>
       <c r="P9" s="2">
-        <v>18.55</v>
+        <v>-7.2</v>
       </c>
       <c r="Q9" s="2">
-        <v>15.89</v>
+        <v>-1.12</v>
       </c>
       <c r="R9" s="2">
-        <v>245.38</v>
+        <v>-2.6</v>
       </c>
       <c r="S9" s="2">
-        <v>51.02</v>
+        <v>-0.57</v>
       </c>
       <c r="T9" s="2">
-        <v>10.37</v>
+        <v>-1.69</v>
       </c>
       <c r="U9" s="2">
-        <v>272.95</v>
+        <v>-0.65</v>
       </c>
       <c r="V9" s="2">
-        <v>57.92</v>
+        <v>-1.75</v>
       </c>
       <c r="W9" s="2">
-        <v>56.06</v>
+        <v>-1.56</v>
       </c>
       <c r="X9" s="2">
-        <v>47.5</v>
-      </c>
-      <c r="Y9" s="2">
-        <v>85.21</v>
-      </c>
-      <c r="Z9" s="2">
-        <v>45.39</v>
+        <v>-3.2</v>
       </c>
     </row>
-    <row r="10" spans="1:26">
+    <row r="10" spans="1:24">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>6.04</v>
+        <v>1.1</v>
       </c>
       <c r="C10" s="2">
-        <v>8.8</v>
+        <v>0.44</v>
       </c>
       <c r="D10" s="2">
-        <v>5.64</v>
+        <v>0.43</v>
       </c>
       <c r="E10" s="2">
-        <v>32.35</v>
+        <v>1.41</v>
       </c>
       <c r="F10" s="2">
-        <v>2.52</v>
+        <v>0.14</v>
       </c>
       <c r="G10" s="2">
-        <v>2.88</v>
+        <v>1.13</v>
       </c>
       <c r="H10" s="2">
-        <v>6.64</v>
+        <v>0.89</v>
       </c>
       <c r="I10" s="2">
-        <v>3.05</v>
+        <v>1.11</v>
       </c>
       <c r="J10" s="2">
-        <v>10.62</v>
+        <v>1.08</v>
       </c>
       <c r="K10" s="2">
-        <v>3.78</v>
+        <v>1.04</v>
       </c>
       <c r="L10" s="2">
-        <v>5.83</v>
+        <v>0.29</v>
       </c>
       <c r="M10" s="2">
-        <v>11.15</v>
+        <v>0.17</v>
       </c>
       <c r="N10" s="2">
-        <v>4.21</v>
+        <v>0.83</v>
       </c>
       <c r="O10" s="2">
-        <v>3.99</v>
+        <v>0.13</v>
       </c>
       <c r="P10" s="2">
-        <v>5.77</v>
+        <v>1.22</v>
       </c>
       <c r="Q10" s="2">
-        <v>2.34</v>
+        <v>0.96</v>
       </c>
       <c r="R10" s="2">
-        <v>2.31</v>
+        <v>1.31</v>
       </c>
       <c r="S10" s="2">
-        <v>2.01</v>
+        <v>0.7</v>
       </c>
       <c r="T10" s="2">
-        <v>2.28</v>
+        <v>0.17</v>
       </c>
       <c r="U10" s="2">
-        <v>4.82</v>
+        <v>0.1</v>
       </c>
       <c r="V10" s="2">
-        <v>40.37</v>
+        <v>0.54</v>
       </c>
       <c r="W10" s="2">
-        <v>8.01</v>
+        <v>0.66</v>
       </c>
       <c r="X10" s="2">
-        <v>2.74</v>
-      </c>
-      <c r="Y10" s="2">
-        <v>6.82</v>
-      </c>
-      <c r="Z10" s="2">
-        <v>2.85</v>
+        <v>0.81</v>
       </c>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:24">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>1.24</v>
+        <v>0.19</v>
       </c>
       <c r="C11" s="2">
-        <v>3.91</v>
+        <v>0.08</v>
       </c>
       <c r="D11" s="2">
-        <v>2.95</v>
+        <v>0.21</v>
       </c>
       <c r="E11" s="2">
-        <v>32.16</v>
+        <v>0.13</v>
       </c>
       <c r="F11" s="2">
-        <v>2.15</v>
+        <v>0.03</v>
       </c>
       <c r="G11" s="2">
-        <v>1.84</v>
+        <v>0.08</v>
       </c>
       <c r="H11" s="2">
-        <v>3.65</v>
+        <v>0.25</v>
       </c>
       <c r="I11" s="2">
-        <v>1.55</v>
+        <v>0.23</v>
       </c>
       <c r="J11" s="2">
-        <v>1.33</v>
+        <v>0.37</v>
       </c>
       <c r="K11" s="2">
-        <v>1.85</v>
+        <v>0.15</v>
       </c>
       <c r="L11" s="2">
-        <v>2.44</v>
+        <v>0.07</v>
       </c>
       <c r="M11" s="2">
-        <v>9.64</v>
+        <v>0.04</v>
       </c>
       <c r="N11" s="2">
-        <v>3.03</v>
+        <v>0.3</v>
       </c>
       <c r="O11" s="2">
-        <v>1.53</v>
+        <v>0.02</v>
       </c>
       <c r="P11" s="2">
-        <v>1.25</v>
+        <v>0.2</v>
       </c>
       <c r="Q11" s="2">
-        <v>1.92</v>
+        <v>0.36</v>
       </c>
       <c r="R11" s="2">
-        <v>2.27</v>
+        <v>0.39</v>
       </c>
       <c r="S11" s="2">
-        <v>1.39</v>
+        <v>0.05</v>
       </c>
       <c r="T11" s="2">
-        <v>1.81</v>
+        <v>0.01</v>
       </c>
       <c r="U11" s="2">
-        <v>1.08</v>
+        <v>0.02</v>
       </c>
       <c r="V11" s="2">
-        <v>9.93</v>
+        <v>0.11</v>
       </c>
       <c r="W11" s="2">
-        <v>7.25</v>
+        <v>0.1</v>
       </c>
       <c r="X11" s="2">
-        <v>2.41</v>
-      </c>
-      <c r="Y11" s="2">
-        <v>3.29</v>
-      </c>
-      <c r="Z11" s="2">
-        <v>1.61</v>
+        <v>0.05</v>
       </c>
     </row>
-    <row r="12" spans="1:26">
+    <row r="12" spans="1:24">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="2">
-        <v>11437.33</v>
+        <v>300.38</v>
       </c>
       <c r="C12" s="2">
-        <v>7680.43</v>
+        <v>822.31</v>
       </c>
       <c r="D12" s="2">
-        <v>45530</v>
+        <v>580.49</v>
       </c>
       <c r="E12" s="2">
-        <v>123597</v>
+        <v>15.68</v>
       </c>
       <c r="F12" s="2">
-        <v>102571</v>
+        <v>178.85</v>
       </c>
       <c r="G12" s="2">
-        <v>19510.14</v>
+        <v>1067.01</v>
       </c>
       <c r="H12" s="2">
-        <v>10187.24</v>
+        <v>1105.81</v>
       </c>
       <c r="I12" s="2">
-        <v>4712.34</v>
+        <v>855.2</v>
       </c>
       <c r="J12" s="2">
-        <v>3026.46</v>
+        <v>373.21</v>
       </c>
       <c r="K12" s="2">
-        <v>12789.81</v>
+        <v>1395.87</v>
       </c>
       <c r="L12" s="2">
-        <v>13314.77</v>
+        <v>1336.31</v>
       </c>
       <c r="M12" s="2">
-        <v>8559.67</v>
+        <v>277.16</v>
       </c>
       <c r="N12" s="2">
-        <v>6690.94</v>
+        <v>1579.84</v>
       </c>
       <c r="O12" s="2">
-        <v>118558</v>
+        <v>1072.47</v>
       </c>
       <c r="P12" s="2">
-        <v>263096</v>
+        <v>1751.63</v>
       </c>
       <c r="Q12" s="2">
-        <v>68172</v>
+        <v>635.46</v>
       </c>
       <c r="R12" s="2">
-        <v>6616.02</v>
+        <v>1999.28</v>
       </c>
       <c r="S12" s="2">
-        <v>4385.59</v>
+        <v>164.47</v>
       </c>
       <c r="T12" s="2">
-        <v>13074.4</v>
+        <v>-86.28</v>
       </c>
       <c r="U12" s="2">
-        <v>4839.36</v>
+        <v>390.23</v>
       </c>
       <c r="V12" s="2">
-        <v>5041.96</v>
+        <v>552.67</v>
       </c>
       <c r="W12" s="2">
-        <v>4102.28</v>
+        <v>263.36</v>
       </c>
       <c r="X12" s="2">
-        <v>14183.04</v>
-      </c>
-      <c r="Y12" s="2">
-        <v>42483.32</v>
-      </c>
-      <c r="Z12" s="2">
-        <v>31472</v>
+        <v>389.6</v>
       </c>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:24">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="1">
-        <v>4.3</v>
+        <v>34.57</v>
       </c>
       <c r="C13" s="1">
-        <v>2.58</v>
+        <v>63.18</v>
       </c>
       <c r="D13" s="1">
-        <v>8.43</v>
+        <v>49.73</v>
       </c>
       <c r="E13" s="1">
-        <v>6.95</v>
+        <v>89.72</v>
       </c>
       <c r="F13" s="1">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="G13" s="1">
-        <v>2.86</v>
+        <v>18.94</v>
       </c>
       <c r="H13" s="1">
-        <v>0.16</v>
+        <v>23.77</v>
       </c>
       <c r="I13" s="1">
-        <v>4.43</v>
+        <v>9.91</v>
       </c>
       <c r="J13" s="1">
-        <v>7.17</v>
+        <v>20.23</v>
       </c>
       <c r="K13" s="1">
-        <v>7.54</v>
+        <v>37.19</v>
       </c>
       <c r="L13" s="1">
-        <v>0.07</v>
+        <v>38.74</v>
       </c>
       <c r="M13" s="1">
-        <v>0.31</v>
+        <v>58.24</v>
       </c>
       <c r="N13" s="1">
-        <v>7.38</v>
+        <v>28.17</v>
       </c>
       <c r="O13" s="1">
-        <v>4.26</v>
+        <v>29.01</v>
       </c>
       <c r="P13" s="1">
-        <v>16.4</v>
+        <v>23.7</v>
       </c>
       <c r="Q13" s="1">
-        <v>6.17</v>
+        <v>17.25</v>
       </c>
       <c r="R13" s="1">
-        <v>1.19</v>
+        <v>31.92</v>
       </c>
       <c r="S13" s="1">
-        <v>1.54</v>
+        <v>61.32</v>
       </c>
       <c r="T13" s="1">
-        <v>23.53</v>
+        <v>103.07</v>
       </c>
       <c r="U13" s="1">
-        <v>7.19</v>
+        <v>65.66</v>
       </c>
       <c r="V13" s="1">
-        <v>1.83</v>
+        <v>44.4</v>
       </c>
       <c r="W13" s="1">
-        <v>1.94</v>
+        <v>20.6</v>
       </c>
       <c r="X13" s="1">
-        <v>8.39</v>
-      </c>
-      <c r="Y13" s="1">
-        <v>8.16</v>
-      </c>
-      <c r="Z13" s="1">
-        <v>13.99</v>
+        <v>36.82</v>
       </c>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:24">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="1">
-        <v>4.77</v>
+        <v>1183.92</v>
       </c>
       <c r="C14" s="1">
-        <v>3.06</v>
+        <v>1056.9</v>
       </c>
       <c r="D14" s="1">
-        <v>10.23</v>
+        <v>123.18</v>
       </c>
       <c r="E14" s="1">
-        <v>7.61</v>
+        <v>6394.05</v>
       </c>
       <c r="F14" s="1">
-        <v>16.75</v>
+        <v>0</v>
       </c>
       <c r="G14" s="1">
-        <v>3.26</v>
+        <v>59.56</v>
       </c>
       <c r="H14" s="1">
-        <v>0.18</v>
+        <v>44.2</v>
       </c>
       <c r="I14" s="1">
-        <v>5.31</v>
+        <v>28.88</v>
       </c>
       <c r="J14" s="1">
-        <v>10.45</v>
+        <v>61.85</v>
       </c>
       <c r="K14" s="1">
-        <v>9.56</v>
+        <v>80.1</v>
       </c>
       <c r="L14" s="1">
-        <v>0.07</v>
+        <v>616.37</v>
       </c>
       <c r="M14" s="1">
-        <v>0.37</v>
+        <v>952.94</v>
       </c>
       <c r="N14" s="1">
-        <v>8.82</v>
+        <v>51.09</v>
       </c>
       <c r="O14" s="1">
-        <v>5.09</v>
+        <v>49.66</v>
       </c>
       <c r="P14" s="1">
-        <v>23.18</v>
+        <v>42.79</v>
       </c>
       <c r="Q14" s="1">
-        <v>7.13</v>
+        <v>35.85</v>
       </c>
       <c r="R14" s="1">
-        <v>1.23</v>
+        <v>66</v>
       </c>
       <c r="S14" s="1">
-        <v>1.6</v>
+        <v>1309.12</v>
       </c>
       <c r="T14" s="1">
-        <v>34.34</v>
+        <v>-410.58</v>
       </c>
       <c r="U14" s="1">
-        <v>8.99</v>
+        <v>386.53</v>
       </c>
       <c r="V14" s="1">
-        <v>2.01</v>
+        <v>149.76</v>
       </c>
       <c r="W14" s="1">
-        <v>2.13</v>
+        <v>123.47</v>
       </c>
       <c r="X14" s="1">
-        <v>10.03</v>
-      </c>
-      <c r="Y14" s="1">
-        <v>9.73</v>
-      </c>
-      <c r="Z14" s="1">
-        <v>24.06</v>
+        <v>76.3</v>
       </c>
     </row>
-    <row r="15" spans="1:26">
+    <row r="15" spans="1:24">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="2">
-        <v>13133.84</v>
+        <v>16209.91</v>
       </c>
       <c r="C15" s="2">
-        <v>9834.97</v>
+        <v>16270.57</v>
       </c>
       <c r="D15" s="2">
-        <v>54955.5</v>
+        <v>1712.82</v>
       </c>
       <c r="E15" s="2">
-        <v>135816</v>
+        <v>630.13</v>
       </c>
       <c r="F15" s="2">
-        <v>129086</v>
+        <v>314.62</v>
       </c>
       <c r="G15" s="2">
-        <v>21423.95</v>
+        <v>3366.76</v>
       </c>
       <c r="H15" s="2">
-        <v>11243.54</v>
+        <v>2143.33</v>
       </c>
       <c r="I15" s="2">
-        <v>5870.42</v>
+        <v>2751.22</v>
       </c>
       <c r="J15" s="2">
-        <v>3504.02</v>
+        <v>1115.49</v>
       </c>
       <c r="K15" s="2">
-        <v>15353.61</v>
+        <v>3308.13</v>
       </c>
       <c r="L15" s="2">
-        <v>14186.39</v>
+        <v>23575.02</v>
       </c>
       <c r="M15" s="2">
-        <v>7990.07</v>
+        <v>5488.21</v>
       </c>
       <c r="N15" s="2">
-        <v>7540.83</v>
+        <v>2898.05</v>
       </c>
       <c r="O15" s="2">
-        <v>139366</v>
+        <v>1703.85</v>
       </c>
       <c r="P15" s="2">
-        <v>276358</v>
+        <v>3005.63</v>
       </c>
       <c r="Q15" s="2">
-        <v>78905.5</v>
+        <v>1566.18</v>
       </c>
       <c r="R15" s="2">
-        <v>6593.88</v>
+        <v>4370.64</v>
       </c>
       <c r="S15" s="2">
-        <v>4480.78</v>
+        <v>3702.27</v>
       </c>
       <c r="T15" s="2">
-        <v>18513.64</v>
+        <v>420.25</v>
       </c>
       <c r="U15" s="2">
-        <v>5793.91</v>
+        <v>2300</v>
       </c>
       <c r="V15" s="2">
-        <v>5040.54</v>
+        <v>1958.95</v>
       </c>
       <c r="W15" s="2">
-        <v>4292.75</v>
+        <v>1671.56</v>
       </c>
       <c r="X15" s="2">
-        <v>17104.8</v>
-      </c>
-      <c r="Y15" s="2">
-        <v>40377.25</v>
-      </c>
-      <c r="Z15" s="2">
-        <v>50862.5</v>
+        <v>634.61</v>
       </c>
     </row>
-    <row r="16" spans="1:26">
+    <row r="16" spans="1:24">
       <c r="A16" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="2">
-        <v>11944.58</v>
+        <v>3189.66</v>
       </c>
       <c r="C16" s="2">
-        <v>8270.26</v>
+        <v>3176.4</v>
       </c>
       <c r="D16" s="2">
-        <v>47848.5</v>
+        <v>701.87</v>
       </c>
       <c r="E16" s="2">
-        <v>123342.5</v>
+        <v>43.58</v>
       </c>
       <c r="F16" s="2">
-        <v>106152.5</v>
+        <v>182.65</v>
       </c>
       <c r="G16" s="2">
-        <v>19229.91</v>
+        <v>1272.21</v>
       </c>
       <c r="H16" s="2">
-        <v>9967.13</v>
+        <v>1211.72</v>
       </c>
       <c r="I16" s="2">
-        <v>4581.34</v>
+        <v>1556.84</v>
       </c>
       <c r="J16" s="2">
-        <v>3310.41</v>
+        <v>393.58</v>
       </c>
       <c r="K16" s="2">
-        <v>12399.85</v>
+        <v>1628.88</v>
       </c>
       <c r="L16" s="2">
-        <v>12358.65</v>
+        <v>2231.67</v>
       </c>
       <c r="M16" s="2">
-        <v>7108.14</v>
+        <v>979.21</v>
       </c>
       <c r="N16" s="2">
-        <v>6138.41</v>
+        <v>1686.93</v>
       </c>
       <c r="O16" s="2">
-        <v>115987.5</v>
+        <v>890.95</v>
       </c>
       <c r="P16" s="2">
-        <v>193439.5</v>
+        <v>2010.25</v>
       </c>
       <c r="Q16" s="2">
-        <v>70748.5</v>
+        <v>922.17</v>
       </c>
       <c r="R16" s="2">
-        <v>6327.29</v>
+        <v>2430.36</v>
       </c>
       <c r="S16" s="2">
-        <v>4324.45</v>
+        <v>203.33</v>
       </c>
       <c r="T16" s="2">
-        <v>13071.56</v>
+        <v>2.65</v>
       </c>
       <c r="U16" s="2">
-        <v>4352.28</v>
+        <v>671.47</v>
       </c>
       <c r="V16" s="2">
-        <v>4730.41</v>
+        <v>711.42</v>
       </c>
       <c r="W16" s="2">
-        <v>3757.47</v>
+        <v>407.92</v>
       </c>
       <c r="X16" s="2">
-        <v>13811.17</v>
-      </c>
-      <c r="Y16" s="2">
-        <v>34002.22</v>
-      </c>
-      <c r="Z16" s="2">
-        <v>36465.5</v>
+        <v>347.11</v>
       </c>
     </row>
-    <row r="17" spans="1:26">
+    <row r="17" spans="1:24">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="1">
-        <v>7.34</v>
+        <v>-22.78</v>
       </c>
       <c r="C17" s="1">
-        <v>13.54</v>
+        <v>-20.72</v>
       </c>
       <c r="D17" s="1">
-        <v>5.16</v>
+        <v>-25.51</v>
       </c>
       <c r="E17" s="1">
-        <v>5.69</v>
+        <v>-19.83</v>
       </c>
       <c r="F17" s="1">
-        <v>8.65</v>
+        <v>-11.15</v>
       </c>
       <c r="G17" s="1">
-        <v>10.89</v>
+        <v>-7</v>
       </c>
       <c r="H17" s="1">
-        <v>12.9</v>
+        <v>-4.55</v>
       </c>
       <c r="I17" s="1">
-        <v>22.61</v>
+        <v>-9.06</v>
       </c>
       <c r="J17" s="1">
-        <v>10.19</v>
+        <v>-10.03</v>
       </c>
       <c r="K17" s="1">
-        <v>8.7</v>
+        <v>-11.4</v>
       </c>
       <c r="L17" s="1">
-        <v>17.45</v>
+        <v>-14.21</v>
       </c>
       <c r="M17" s="1">
-        <v>8.12</v>
+        <v>-26.74</v>
       </c>
       <c r="N17" s="1">
-        <v>6.38</v>
+        <v>-6.23</v>
       </c>
       <c r="O17" s="1">
-        <v>6.72</v>
+        <v>-8.74</v>
       </c>
       <c r="P17" s="1">
-        <v>6.19</v>
+        <v>-14.08</v>
       </c>
       <c r="Q17" s="1">
-        <v>3.68</v>
+        <v>-17.16</v>
       </c>
       <c r="R17" s="1">
-        <v>8.1</v>
+        <v>-8.3</v>
       </c>
       <c r="S17" s="1">
-        <v>3.85</v>
+        <v>-3.11</v>
       </c>
       <c r="T17" s="1">
-        <v>7.76</v>
+        <v>-42.95</v>
       </c>
       <c r="U17" s="1">
-        <v>8</v>
+        <v>-8.04</v>
       </c>
       <c r="V17" s="1">
-        <v>14.15</v>
+        <v>-18.23</v>
       </c>
       <c r="W17" s="1">
-        <v>8.61</v>
+        <v>-11.51</v>
       </c>
       <c r="X17" s="1">
-        <v>7.92</v>
-      </c>
-      <c r="Y17" s="1">
-        <v>40.71</v>
-      </c>
-      <c r="Z17" s="1">
-        <v>7.68</v>
+        <v>-14.13</v>
       </c>
     </row>
-    <row r="18" spans="1:26">
+    <row r="18" spans="1:24">
       <c r="A18" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="2">
-        <v>1.1</v>
+        <v>5.08</v>
       </c>
       <c r="C18" s="2">
-        <v>1.19</v>
+        <v>5.12</v>
       </c>
       <c r="D18" s="2">
-        <v>1.15</v>
+        <v>2.44</v>
       </c>
       <c r="E18" s="2">
-        <v>1.1</v>
+        <v>14.46</v>
       </c>
       <c r="F18" s="2">
-        <v>1.22</v>
+        <v>1.72</v>
       </c>
       <c r="G18" s="2">
-        <v>1.11</v>
+        <v>2.65</v>
       </c>
       <c r="H18" s="2">
-        <v>1.13</v>
+        <v>1.77</v>
       </c>
       <c r="I18" s="2">
-        <v>1.28</v>
+        <v>1.77</v>
       </c>
       <c r="J18" s="2">
-        <v>1.06</v>
+        <v>2.83</v>
       </c>
       <c r="K18" s="2">
-        <v>1.24</v>
+        <v>2.03</v>
       </c>
       <c r="L18" s="2">
-        <v>1.15</v>
+        <v>10.56</v>
       </c>
       <c r="M18" s="2">
-        <v>1.12</v>
+        <v>5.6</v>
       </c>
       <c r="N18" s="2">
-        <v>1.23</v>
+        <v>1.72</v>
       </c>
       <c r="O18" s="2">
-        <v>1.2</v>
+        <v>1.91</v>
       </c>
       <c r="P18" s="2">
-        <v>1.43</v>
+        <v>1.5</v>
       </c>
       <c r="Q18" s="2">
-        <v>1.12</v>
+        <v>1.7</v>
       </c>
       <c r="R18" s="2">
-        <v>1.04</v>
+        <v>1.8</v>
       </c>
       <c r="S18" s="2">
-        <v>1.04</v>
+        <v>18.21</v>
       </c>
       <c r="T18" s="2">
-        <v>1.42</v>
+        <v>158.55</v>
       </c>
       <c r="U18" s="2">
-        <v>1.33</v>
+        <v>3.43</v>
       </c>
       <c r="V18" s="2">
-        <v>1.07</v>
+        <v>2.75</v>
       </c>
       <c r="W18" s="2">
-        <v>1.14</v>
+        <v>4.1</v>
       </c>
       <c r="X18" s="2">
-        <v>1.24</v>
-      </c>
-      <c r="Y18" s="2">
-        <v>1.19</v>
-      </c>
-      <c r="Z18" s="2">
-        <v>1.39</v>
+        <v>1.83</v>
       </c>
     </row>
-    <row r="19" spans="1:26">
+    <row r="19" spans="1:24">
       <c r="A19" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="1">
-        <v>5.57</v>
+        <v>6.13</v>
       </c>
       <c r="C19" s="1">
-        <v>4.27</v>
+        <v>38.72</v>
       </c>
       <c r="D19" s="1">
-        <v>11.16</v>
+        <v>50.06</v>
       </c>
       <c r="E19" s="1">
-        <v>7.21</v>
+        <v>187.01</v>
       </c>
       <c r="F19" s="1">
-        <v>16.69</v>
+        <v>0.68</v>
       </c>
       <c r="G19" s="1">
-        <v>4.89</v>
+        <v>3.54</v>
       </c>
       <c r="H19" s="1">
-        <v>7.34</v>
+        <v>0.24</v>
       </c>
       <c r="I19" s="1">
-        <v>6.55</v>
+        <v>4.23</v>
       </c>
       <c r="J19" s="1">
-        <v>4.09</v>
+        <v>3.01</v>
       </c>
       <c r="K19" s="1">
-        <v>3.09</v>
+        <v>3.13</v>
       </c>
       <c r="L19" s="1">
-        <v>18.52</v>
+        <v>41.4</v>
       </c>
       <c r="M19" s="1">
-        <v>5.75</v>
+        <v>2639.57</v>
       </c>
       <c r="N19" s="1">
-        <v>3.37</v>
+        <v>0.07</v>
       </c>
       <c r="O19" s="1">
-        <v>3.62</v>
+        <v>42.56</v>
       </c>
       <c r="P19" s="1">
-        <v>3.93</v>
+        <v>8.78</v>
       </c>
       <c r="Q19" s="1">
-        <v>3.88</v>
+        <v>3.91</v>
       </c>
       <c r="R19" s="1">
-        <v>11.81</v>
+        <v>1.15</v>
       </c>
       <c r="S19" s="1">
-        <v>3.15</v>
+        <v>12.57</v>
       </c>
       <c r="T19" s="1">
-        <v>19.58</v>
+        <v>16031.53</v>
       </c>
       <c r="U19" s="1">
-        <v>10.14</v>
+        <v>55.5</v>
       </c>
       <c r="V19" s="1">
-        <v>124.56</v>
+        <v>23.63</v>
       </c>
       <c r="W19" s="1">
-        <v>7.26</v>
+        <v>5.2</v>
       </c>
       <c r="X19" s="1">
-        <v>4.85</v>
-      </c>
-      <c r="Y19" s="1">
-        <v>154.03</v>
-      </c>
-      <c r="Z19" s="1">
-        <v>7.21</v>
+        <v>5.43</v>
       </c>
     </row>
-    <row r="20" spans="1:26">
+    <row r="20" spans="1:24">
       <c r="A20" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="2">
-        <v>10.54</v>
+        <v>1.31</v>
       </c>
       <c r="C20" s="2">
-        <v>29.06</v>
+        <v>0.77</v>
       </c>
       <c r="D20" s="2">
-        <v>2.83</v>
+        <v>1.48</v>
       </c>
       <c r="E20" s="2">
-        <v>10.09</v>
+        <v>1.28</v>
       </c>
       <c r="F20" s="2">
-        <v>6.72</v>
+        <v>-0.05</v>
       </c>
       <c r="G20" s="2">
-        <v>28.66</v>
+        <v>1.24</v>
       </c>
       <c r="H20" s="2">
-        <v>307.3</v>
+        <v>0.94</v>
       </c>
       <c r="I20" s="2">
-        <v>55.38</v>
+        <v>1.91</v>
       </c>
       <c r="J20" s="2">
-        <v>8.98</v>
+        <v>1.71</v>
       </c>
       <c r="K20" s="2">
-        <v>5.27</v>
+        <v>1.04</v>
       </c>
       <c r="L20" s="2">
-        <v>1200.01</v>
+        <v>0.19</v>
       </c>
       <c r="M20" s="2">
-        <v>94.76</v>
+        <v>0.3</v>
       </c>
       <c r="N20" s="2">
-        <v>2.04</v>
+        <v>1.65</v>
       </c>
       <c r="O20" s="2">
-        <v>8.02</v>
+        <v>0.84</v>
       </c>
       <c r="P20" s="2">
-        <v>2.66</v>
+        <v>1.54</v>
       </c>
       <c r="Q20" s="2">
-        <v>4.18</v>
+        <v>1.57</v>
       </c>
       <c r="R20" s="2">
-        <v>18.7</v>
+        <v>1.43</v>
       </c>
       <c r="S20" s="2">
-        <v>11.14</v>
+        <v>0.13</v>
       </c>
       <c r="T20" s="2">
-        <v>2.2</v>
+        <v>0.82</v>
       </c>
       <c r="U20" s="2">
-        <v>2.95</v>
+        <v>0.49</v>
       </c>
       <c r="V20" s="2">
-        <v>11.55</v>
+        <v>1.82</v>
       </c>
       <c r="W20" s="2">
-        <v>8.67</v>
+        <v>0.79</v>
       </c>
       <c r="X20" s="2">
-        <v>3.27</v>
-      </c>
-      <c r="Y20" s="2">
-        <v>21.31</v>
-      </c>
-      <c r="Z20" s="2">
-        <v>6.04</v>
+        <v>1.26</v>
       </c>
     </row>
-    <row r="21" spans="1:26">
+    <row r="21" spans="1:24">
       <c r="A21" t="s">
         <v>20</v>
       </c>
       <c r="B21" s="2">
-        <v>9.26</v>
+        <v>-0.06</v>
       </c>
       <c r="C21" s="2">
-        <v>8.12</v>
+        <v>-0.33</v>
       </c>
       <c r="D21" s="2">
-        <v>7.37</v>
+        <v>-1.42</v>
       </c>
       <c r="E21" s="2">
-        <v>19.05</v>
+        <v>-1.37</v>
       </c>
       <c r="F21" s="2">
-        <v>16.77</v>
+        <v>-1.62</v>
       </c>
       <c r="G21" s="2">
-        <v>12.98</v>
+        <v>-2.91</v>
       </c>
       <c r="H21" s="2">
-        <v>6.35</v>
+        <v>-4.29</v>
       </c>
       <c r="I21" s="2">
-        <v>16.87</v>
+        <v>-1.81</v>
       </c>
       <c r="J21" s="2">
-        <v>12.06</v>
+        <v>-2.34</v>
       </c>
       <c r="K21" s="2">
-        <v>6.71</v>
+        <v>-0.97</v>
       </c>
       <c r="L21" s="2">
-        <v>8.03</v>
+        <v>-0.54</v>
       </c>
       <c r="M21" s="2">
-        <v>7.52</v>
+        <v>-0.55</v>
       </c>
       <c r="N21" s="2">
-        <v>2.76</v>
+        <v>-7.95</v>
       </c>
       <c r="O21" s="2">
-        <v>8.17</v>
+        <v>-4.68</v>
       </c>
       <c r="P21" s="2">
-        <v>10.48</v>
+        <v>-2.15</v>
       </c>
       <c r="Q21" s="2">
-        <v>11.48</v>
+        <v>-1.28</v>
       </c>
       <c r="R21" s="2">
-        <v>4.81</v>
+        <v>-2.81</v>
       </c>
       <c r="S21" s="2">
-        <v>7.55</v>
+        <v>-6.4</v>
       </c>
       <c r="T21" s="2">
-        <v>8.99</v>
+        <v>-0.57</v>
       </c>
       <c r="U21" s="2">
-        <v>3.18</v>
+        <v>-7.12</v>
       </c>
       <c r="V21" s="2">
-        <v>2.6</v>
+        <v>-5.14</v>
       </c>
       <c r="W21" s="2">
-        <v>3.19</v>
+        <v>-0.84</v>
       </c>
       <c r="X21" s="2">
-        <v>5.46</v>
-      </c>
-      <c r="Y21" s="2">
-        <v>9.13</v>
-      </c>
-      <c r="Z21" s="2">
-        <v>18.05</v>
+        <v>-3.03</v>
       </c>
     </row>
-    <row r="22" spans="1:26">
+    <row r="22" spans="1:24">
       <c r="A22" t="s">
         <v>21</v>
       </c>
       <c r="B22" s="2">
-        <v>1.34</v>
+        <v>0.06</v>
       </c>
       <c r="C22" s="2">
-        <v>24.67</v>
+        <v>0.18</v>
       </c>
       <c r="D22" s="2">
-        <v>24.01</v>
+        <v>0.64</v>
       </c>
       <c r="E22" s="2">
-        <v>69.02</v>
+        <v>0.14</v>
       </c>
       <c r="F22" s="2">
-        <v>70.64</v>
+        <v>0.02</v>
       </c>
       <c r="G22" s="2">
-        <v>13.99</v>
+        <v>4.06</v>
       </c>
       <c r="H22" s="2">
-        <v>2.96</v>
+        <v>0.24</v>
       </c>
       <c r="I22" s="2">
-        <v>5.81</v>
+        <v>3.76</v>
       </c>
       <c r="J22" s="2">
-        <v>0.28</v>
+        <v>0.49</v>
       </c>
       <c r="K22" s="2">
-        <v>3.96</v>
+        <v>0.19</v>
       </c>
       <c r="L22" s="2">
-        <v>1.65</v>
+        <v>0.2</v>
       </c>
       <c r="M22" s="2">
-        <v>0.66</v>
+        <v>0.24</v>
       </c>
       <c r="N22" s="2">
-        <v>0.7</v>
+        <v>0.52</v>
       </c>
       <c r="O22" s="2">
-        <v>12.43</v>
+        <v>0.21</v>
       </c>
       <c r="P22" s="2">
-        <v>46.65</v>
+        <v>0.68</v>
       </c>
       <c r="Q22" s="2">
-        <v>31.86</v>
+        <v>0.31</v>
       </c>
       <c r="R22" s="2">
-        <v>3.21</v>
+        <v>0.31</v>
       </c>
       <c r="S22" s="2">
-        <v>11.82</v>
+        <v>0.19</v>
       </c>
       <c r="T22" s="2">
-        <v>18.98</v>
+        <v>0.19</v>
       </c>
       <c r="U22" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="V22" s="2">
         <v>0.22</v>
       </c>
-      <c r="V22" s="2">
-        <v>0.26</v>
-      </c>
       <c r="W22" s="2">
-        <v>0.39</v>
+        <v>0.32</v>
       </c>
       <c r="X22" s="2">
-        <v>12.81</v>
-      </c>
-      <c r="Y22" s="2">
-        <v>2.27</v>
-      </c>
-      <c r="Z22" s="2">
-        <v>11.25</v>
+        <v>0.06</v>
       </c>
     </row>
-    <row r="23" spans="1:26">
+    <row r="23" spans="1:24">
       <c r="A23" t="s">
         <v>22</v>
       </c>
       <c r="B23" s="2">
-        <v>1.69</v>
+        <v>0.08</v>
       </c>
       <c r="C23" s="2">
-        <v>26.75</v>
+        <v>0.18</v>
       </c>
       <c r="D23" s="2">
-        <v>27.25</v>
+        <v>0.73</v>
       </c>
       <c r="E23" s="2">
-        <v>77.4</v>
+        <v>0.1</v>
       </c>
       <c r="F23" s="2">
-        <v>69.25</v>
+        <v>0.02</v>
       </c>
       <c r="G23" s="2">
-        <v>15.24</v>
+        <v>3.06</v>
       </c>
       <c r="H23" s="2">
-        <v>2.88</v>
+        <v>0.33</v>
       </c>
       <c r="I23" s="2">
-        <v>5.77</v>
+        <v>3.2</v>
       </c>
       <c r="J23" s="2">
-        <v>0.3</v>
+        <v>0.41</v>
       </c>
       <c r="K23" s="2">
-        <v>4.78</v>
+        <v>0.22</v>
       </c>
       <c r="L23" s="2">
-        <v>1.75</v>
+        <v>0.24</v>
       </c>
       <c r="M23" s="2">
-        <v>0.47</v>
+        <v>0.24</v>
       </c>
       <c r="N23" s="2">
-        <v>0.75</v>
+        <v>0.51</v>
       </c>
       <c r="O23" s="2">
-        <v>13.62</v>
+        <v>0.2</v>
       </c>
       <c r="P23" s="2">
-        <v>54.8</v>
+        <v>0.57</v>
       </c>
       <c r="Q23" s="2">
-        <v>37.5</v>
+        <v>0.33</v>
       </c>
       <c r="R23" s="2">
-        <v>3.9</v>
+        <v>0.41</v>
       </c>
       <c r="S23" s="2">
-        <v>12.76</v>
+        <v>0.16</v>
       </c>
       <c r="T23" s="2">
-        <v>19.08</v>
+        <v>0.17</v>
       </c>
       <c r="U23" s="2">
-        <v>0.28</v>
+        <v>0.07</v>
       </c>
       <c r="V23" s="2">
-        <v>0.33</v>
+        <v>0.22</v>
       </c>
       <c r="W23" s="2">
-        <v>0.39</v>
+        <v>0.4</v>
       </c>
       <c r="X23" s="2">
-        <v>13.68</v>
-      </c>
-      <c r="Y23" s="2">
-        <v>2.1</v>
-      </c>
-      <c r="Z23" s="2">
-        <v>11.62</v>
+        <v>0.06</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Revert "Major update on the refining some codes""
This reverts commit 13ba4c9d4da19d28410df9dbbdc9a6ed5ff0fb5f.
</commit_message>
<xml_diff>
--- a/Sample Output/highlight.xlsx
+++ b/Sample Output/highlight.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="78">
   <si>
     <t>Original Currency</t>
   </si>
@@ -91,148 +91,163 @@
     <t>Million</t>
   </si>
   <si>
-    <t>2014</t>
-  </si>
-  <si>
-    <t>01733</t>
-  </si>
-  <si>
-    <t>WINSWAY</t>
-  </si>
-  <si>
-    <t>00809</t>
-  </si>
-  <si>
-    <t>GLOBAL BIO-CHEM</t>
-  </si>
-  <si>
     <t>2015</t>
   </si>
   <si>
-    <t>00094</t>
-  </si>
-  <si>
-    <t>GREENHEART GP</t>
-  </si>
-  <si>
-    <t>08163</t>
-  </si>
-  <si>
-    <t>MERDEKA FIN</t>
-  </si>
-  <si>
-    <t>08186</t>
-  </si>
-  <si>
-    <t>IR RESOURCES</t>
-  </si>
-  <si>
-    <t>00300</t>
-  </si>
-  <si>
-    <t>KUNMING MACHINE</t>
-  </si>
-  <si>
-    <t>01198</t>
-  </si>
-  <si>
-    <t>ROYALE FURN</t>
-  </si>
-  <si>
-    <t>00187</t>
-  </si>
-  <si>
-    <t>JINGCHENG MAC</t>
-  </si>
-  <si>
-    <t>00515</t>
-  </si>
-  <si>
-    <t>TC ORI LIGHT</t>
-  </si>
-  <si>
-    <t>00103</t>
-  </si>
-  <si>
-    <t>SHOUGANG CENT</t>
-  </si>
-  <si>
-    <t>00697</t>
-  </si>
-  <si>
-    <t>SHOUGANG INT'L</t>
-  </si>
-  <si>
-    <t>02889</t>
-  </si>
-  <si>
-    <t>NRI HOLDINGS</t>
-  </si>
-  <si>
-    <t>01132</t>
-  </si>
-  <si>
-    <t>ORANGE SKY G H</t>
-  </si>
-  <si>
-    <t>08228</t>
-  </si>
-  <si>
-    <t>NATIONAL ARTS</t>
-  </si>
-  <si>
-    <t>02178</t>
-  </si>
-  <si>
-    <t>PETRO-KING</t>
-  </si>
-  <si>
-    <t>00629</t>
-  </si>
-  <si>
-    <t>YUE DA MINING</t>
-  </si>
-  <si>
-    <t>01080</t>
-  </si>
-  <si>
-    <t>SHENGLI PIPE</t>
-  </si>
-  <si>
-    <t>00760</t>
-  </si>
-  <si>
-    <t>TALENT PPT GP</t>
-  </si>
-  <si>
-    <t>08272</t>
-  </si>
-  <si>
-    <t>C FOOD&amp;BEV; GP</t>
-  </si>
-  <si>
-    <t>00351</t>
-  </si>
-  <si>
-    <t>ASIA ENERGY LOG</t>
-  </si>
-  <si>
-    <t>00402</t>
-  </si>
-  <si>
-    <t>PEACEMAP HOLD</t>
-  </si>
-  <si>
-    <t>08045</t>
-  </si>
-  <si>
-    <t>NANDASOFT</t>
-  </si>
-  <si>
-    <t>00381</t>
-  </si>
-  <si>
-    <t>KIU HUNG INT'L</t>
+    <t>03818</t>
+  </si>
+  <si>
+    <t>CHINA DONGXIANG</t>
+  </si>
+  <si>
+    <t>00511</t>
+  </si>
+  <si>
+    <t>TVB</t>
+  </si>
+  <si>
+    <t>00054</t>
+  </si>
+  <si>
+    <t>HOPEWELL HOLD</t>
+  </si>
+  <si>
+    <t>00006</t>
+  </si>
+  <si>
+    <t>POWER ASSETS</t>
+  </si>
+  <si>
+    <t>01038</t>
+  </si>
+  <si>
+    <t>CKI HOLDINGS</t>
+  </si>
+  <si>
+    <t>00586</t>
+  </si>
+  <si>
+    <t>CONCH VENTURE</t>
+  </si>
+  <si>
+    <t>2016</t>
+  </si>
+  <si>
+    <t>00336</t>
+  </si>
+  <si>
+    <t>HUABAO INTL</t>
+  </si>
+  <si>
+    <t>01999</t>
+  </si>
+  <si>
+    <t>MAN WAH HLDGS</t>
+  </si>
+  <si>
+    <t>00273</t>
+  </si>
+  <si>
+    <t>MASON FIN</t>
+  </si>
+  <si>
+    <t>01066</t>
+  </si>
+  <si>
+    <t>WEIGAO GROUP</t>
+  </si>
+  <si>
+    <t>00460</t>
+  </si>
+  <si>
+    <t>SIHUAN PHARM</t>
+  </si>
+  <si>
+    <t>00587</t>
+  </si>
+  <si>
+    <t>HUA HAN HEALTH</t>
+  </si>
+  <si>
+    <t>02010</t>
+  </si>
+  <si>
+    <t>REAL NUTRI</t>
+  </si>
+  <si>
+    <t>00083</t>
+  </si>
+  <si>
+    <t>SINO LAND</t>
+  </si>
+  <si>
+    <t>01113</t>
+  </si>
+  <si>
+    <t>CK PROPERTY</t>
+  </si>
+  <si>
+    <t>00014</t>
+  </si>
+  <si>
+    <t>HYSAN DEV</t>
+  </si>
+  <si>
+    <t>00075</t>
+  </si>
+  <si>
+    <t>Y.T. REALTY</t>
+  </si>
+  <si>
+    <t>00225</t>
+  </si>
+  <si>
+    <t>POKFULAM</t>
+  </si>
+  <si>
+    <t>00251</t>
+  </si>
+  <si>
+    <t>SEA HOLDINGS</t>
+  </si>
+  <si>
+    <t>00064</t>
+  </si>
+  <si>
+    <t>GET NICE</t>
+  </si>
+  <si>
+    <t>00622</t>
+  </si>
+  <si>
+    <t>ENERCHINA HOLD</t>
+  </si>
+  <si>
+    <t>2013</t>
+  </si>
+  <si>
+    <t>01149</t>
+  </si>
+  <si>
+    <t>ANXIN-CHINA</t>
+  </si>
+  <si>
+    <t>00071</t>
+  </si>
+  <si>
+    <t>MIRAMAR HOTEL</t>
+  </si>
+  <si>
+    <t>00678</t>
+  </si>
+  <si>
+    <t>GENTING HK</t>
+  </si>
+  <si>
+    <t>00270</t>
+  </si>
+  <si>
+    <t>GUANGDONG INV</t>
   </si>
 </sst>
 </file>
@@ -570,7 +585,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X23"/>
+  <dimension ref="A1:Z23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
@@ -580,10 +595,10 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="25" width="15.7109375" customWidth="1"/>
+    <col min="2" max="27" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:26">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -656,8 +671,14 @@
       <c r="X1" t="s">
         <v>23</v>
       </c>
+      <c r="Y1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:26">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -730,8 +751,14 @@
       <c r="X2" t="s">
         <v>24</v>
       </c>
+      <c r="Y2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:26">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -742,37 +769,37 @@
         <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H3" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="I3" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="J3" t="s">
         <v>25</v>
       </c>
       <c r="K3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="L3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="M3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="N3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="O3" t="s">
         <v>25</v>
@@ -784,28 +811,34 @@
         <v>25</v>
       </c>
       <c r="R3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="S3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="T3" t="s">
         <v>25</v>
       </c>
       <c r="U3" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="V3" t="s">
         <v>25</v>
       </c>
       <c r="W3" t="s">
-        <v>30</v>
+        <v>69</v>
       </c>
       <c r="X3" t="s">
-        <v>30</v>
+        <v>25</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:26">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -816,16 +849,16 @@
         <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H4" t="s">
         <v>39</v>
@@ -873,13 +906,19 @@
         <v>67</v>
       </c>
       <c r="W4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="X4" t="s">
-        <v>71</v>
+        <v>72</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:26">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -890,16 +929,16 @@
         <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H5" t="s">
         <v>40</v>
@@ -947,1342 +986,1456 @@
         <v>68</v>
       </c>
       <c r="W5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="X5" t="s">
-        <v>72</v>
+        <v>73</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:26">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>1.35</v>
+        <v>55.48</v>
       </c>
       <c r="C6" s="1">
-        <v>-13.9</v>
+        <v>54.9</v>
       </c>
       <c r="D6" s="1">
-        <v>19.23</v>
+        <v>58.55</v>
       </c>
       <c r="E6" s="1">
-        <v>14.24</v>
+        <v>99.39</v>
       </c>
       <c r="F6" s="1">
-        <v>27.8</v>
+        <v>100</v>
       </c>
       <c r="G6" s="1">
-        <v>15.03</v>
+        <v>37.99</v>
       </c>
       <c r="H6" s="1">
-        <v>16.67</v>
+        <v>68.87</v>
       </c>
       <c r="I6" s="1">
-        <v>5.69</v>
+        <v>39.52</v>
       </c>
       <c r="J6" s="1">
-        <v>7.42</v>
+        <v>100</v>
       </c>
       <c r="K6" s="1">
-        <v>1.29</v>
+        <v>59.4</v>
       </c>
       <c r="L6" s="1">
-        <v>-15.61</v>
+        <v>70.35</v>
       </c>
       <c r="M6" s="1">
-        <v>-220.02</v>
+        <v>68.67</v>
       </c>
       <c r="N6" s="1">
-        <v>57.08</v>
+        <v>65.36</v>
       </c>
       <c r="O6" s="1">
-        <v>100</v>
+        <v>26.56</v>
       </c>
       <c r="P6" s="1">
         <v>100</v>
       </c>
       <c r="Q6" s="1">
-        <v>-7.61</v>
+        <v>87.93</v>
       </c>
       <c r="R6" s="1">
-        <v>1.95</v>
+        <v>97.58</v>
       </c>
       <c r="S6" s="1">
-        <v>21.06</v>
+        <v>62.8</v>
       </c>
       <c r="T6" s="1">
-        <v>0.59</v>
+        <v>100</v>
       </c>
       <c r="U6" s="1">
-        <v>11.07</v>
+        <v>100</v>
       </c>
       <c r="V6" s="1">
-        <v>21.76</v>
+        <v>100</v>
       </c>
       <c r="W6" s="1">
-        <v>13.26</v>
+        <v>78.53</v>
       </c>
       <c r="X6" s="1">
-        <v>35.68</v>
+        <v>63.25</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>100</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>66.99</v>
       </c>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:26">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>-5.3</v>
+        <v>69.1</v>
       </c>
       <c r="C7" s="1">
-        <v>-36.48</v>
+        <v>26.53</v>
       </c>
       <c r="D7" s="1">
-        <v>-80.41</v>
+        <v>188.42</v>
       </c>
       <c r="E7" s="1">
-        <v>-65.23</v>
+        <v>114.98</v>
       </c>
       <c r="F7" s="1">
-        <v>-3.55</v>
+        <v>158.68</v>
       </c>
       <c r="G7" s="1">
-        <v>-19.1</v>
+        <v>40.31</v>
       </c>
       <c r="H7" s="1">
-        <v>-2.99</v>
+        <v>50.44</v>
       </c>
       <c r="I7" s="1">
-        <v>-26.43</v>
+        <v>22.62</v>
       </c>
       <c r="J7" s="1">
-        <v>-10.59</v>
+        <v>37.93</v>
       </c>
       <c r="K7" s="1">
-        <v>-13.51</v>
+        <v>28.66</v>
       </c>
       <c r="L7" s="1">
-        <v>-27.58</v>
+        <v>92.46</v>
       </c>
       <c r="M7" s="1">
-        <v>-1761.3</v>
+        <v>63</v>
       </c>
       <c r="N7" s="1">
-        <v>-0.61</v>
+        <v>42.94</v>
       </c>
       <c r="O7" s="1">
-        <v>-254.61</v>
+        <v>44.81</v>
       </c>
       <c r="P7" s="1">
-        <v>-41.7</v>
+        <v>44.47</v>
       </c>
       <c r="Q7" s="1">
-        <v>-13.41</v>
+        <v>94.49</v>
       </c>
       <c r="R7" s="1">
-        <v>-7.73</v>
+        <v>139.81</v>
       </c>
       <c r="S7" s="1">
-        <v>-22.2</v>
+        <v>79.1</v>
       </c>
       <c r="T7" s="1">
-        <v>-235.44</v>
+        <v>178.28</v>
       </c>
       <c r="U7" s="1">
-        <v>-201.64</v>
+        <v>95.19</v>
       </c>
       <c r="V7" s="1">
-        <v>-47.06</v>
+        <v>826.32</v>
       </c>
       <c r="W7" s="1">
-        <v>-11.02</v>
+        <v>73.87</v>
       </c>
       <c r="X7" s="1">
-        <v>-21.02</v>
+        <v>49.42</v>
+      </c>
+      <c r="Y7" s="1">
+        <v>318.64</v>
+      </c>
+      <c r="Z7" s="1">
+        <v>67.3</v>
       </c>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:26">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>-48.93</v>
+        <v>54.66</v>
       </c>
       <c r="C8" s="1">
-        <v>-52.68</v>
+        <v>29.88</v>
       </c>
       <c r="D8" s="1">
-        <v>-73.88</v>
+        <v>152.01</v>
       </c>
       <c r="E8" s="1">
-        <v>-95.09</v>
+        <v>591.13</v>
       </c>
       <c r="F8" s="1">
-        <v>-90.16</v>
+        <v>183.16</v>
       </c>
       <c r="G8" s="1">
-        <v>-25.29</v>
+        <v>94.5</v>
       </c>
       <c r="H8" s="1">
-        <v>-14.77</v>
+        <v>36.92</v>
       </c>
       <c r="I8" s="1">
-        <v>-19.3</v>
+        <v>18.11</v>
       </c>
       <c r="J8" s="1">
-        <v>-15.85</v>
+        <v>209.94</v>
       </c>
       <c r="K8" s="1">
-        <v>-25.46</v>
+        <v>18.8</v>
       </c>
       <c r="L8" s="1">
-        <v>-46.05</v>
+        <v>65.12</v>
       </c>
       <c r="M8" s="1">
-        <v>-3160.23</v>
+        <v>35.63</v>
       </c>
       <c r="N8" s="1">
-        <v>-14.13</v>
+        <v>19.55</v>
       </c>
       <c r="O8" s="1">
-        <v>-646.32</v>
+        <v>42.91</v>
       </c>
       <c r="P8" s="1">
-        <v>-59.96</v>
+        <v>29.58</v>
       </c>
       <c r="Q8" s="1">
-        <v>-166.19</v>
+        <v>84.64</v>
       </c>
       <c r="R8" s="1">
-        <v>-15.46</v>
+        <v>244.34</v>
       </c>
       <c r="S8" s="1">
-        <v>-31.46</v>
+        <v>130.17</v>
       </c>
       <c r="T8" s="1">
-        <v>-385.88</v>
+        <v>195.98</v>
       </c>
       <c r="U8" s="1">
-        <v>-503.85</v>
+        <v>79.78</v>
       </c>
       <c r="V8" s="1">
-        <v>-107.01</v>
+        <v>657.49</v>
       </c>
       <c r="W8" s="1">
-        <v>-31.26</v>
+        <v>55.01</v>
       </c>
       <c r="X8" s="1">
-        <v>-40.15</v>
+        <v>41.69</v>
+      </c>
+      <c r="Y8" s="1">
+        <v>306.21</v>
+      </c>
+      <c r="Z8" s="1">
+        <v>42.58</v>
       </c>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:26">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>-1.15</v>
+        <v>0</v>
       </c>
       <c r="C9" s="2">
-        <v>-2.99</v>
+        <v>183.51</v>
       </c>
       <c r="D9" s="2">
-        <v>-13</v>
+        <v>36.6</v>
       </c>
       <c r="E9" s="2">
-        <v>-5.19</v>
+        <v>5.7</v>
       </c>
       <c r="F9" s="2">
-        <v>-0.05</v>
+        <v>13.32</v>
       </c>
       <c r="G9" s="2">
-        <v>-3.35</v>
+        <v>21.56</v>
       </c>
       <c r="H9" s="2">
-        <v>-0.83</v>
+        <v>157.79</v>
       </c>
       <c r="I9" s="2">
-        <v>-20.85</v>
+        <v>138.53</v>
       </c>
       <c r="J9" s="2">
-        <v>-8.19</v>
+        <v>23.19</v>
       </c>
       <c r="K9" s="2">
-        <v>-4.07</v>
+        <v>35.7</v>
       </c>
       <c r="L9" s="2">
-        <v>-4.21</v>
+        <v>18302.44</v>
       </c>
       <c r="M9" s="2">
-        <v>-1.51</v>
+        <v>30.12</v>
       </c>
       <c r="N9" s="2">
-        <v>-0.18</v>
+        <v>16.32</v>
       </c>
       <c r="O9" s="2">
-        <v>-0.72</v>
+        <v>40.95</v>
       </c>
       <c r="P9" s="2">
-        <v>-7.2</v>
+        <v>18.55</v>
       </c>
       <c r="Q9" s="2">
-        <v>-1.12</v>
+        <v>15.89</v>
       </c>
       <c r="R9" s="2">
-        <v>-2.6</v>
+        <v>245.38</v>
       </c>
       <c r="S9" s="2">
-        <v>-0.57</v>
+        <v>51.02</v>
       </c>
       <c r="T9" s="2">
-        <v>-1.69</v>
+        <v>10.37</v>
       </c>
       <c r="U9" s="2">
-        <v>-0.65</v>
+        <v>272.95</v>
       </c>
       <c r="V9" s="2">
-        <v>-1.75</v>
+        <v>57.92</v>
       </c>
       <c r="W9" s="2">
-        <v>-1.56</v>
+        <v>56.06</v>
       </c>
       <c r="X9" s="2">
-        <v>-3.2</v>
+        <v>47.5</v>
+      </c>
+      <c r="Y9" s="2">
+        <v>85.21</v>
+      </c>
+      <c r="Z9" s="2">
+        <v>45.39</v>
       </c>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:26">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>1.1</v>
+        <v>6.04</v>
       </c>
       <c r="C10" s="2">
-        <v>0.44</v>
+        <v>8.8</v>
       </c>
       <c r="D10" s="2">
-        <v>0.43</v>
+        <v>5.64</v>
       </c>
       <c r="E10" s="2">
-        <v>1.41</v>
+        <v>32.35</v>
       </c>
       <c r="F10" s="2">
-        <v>0.14</v>
+        <v>2.52</v>
       </c>
       <c r="G10" s="2">
-        <v>1.13</v>
+        <v>2.88</v>
       </c>
       <c r="H10" s="2">
-        <v>0.89</v>
+        <v>6.64</v>
       </c>
       <c r="I10" s="2">
-        <v>1.11</v>
+        <v>3.05</v>
       </c>
       <c r="J10" s="2">
-        <v>1.08</v>
+        <v>10.62</v>
       </c>
       <c r="K10" s="2">
-        <v>1.04</v>
+        <v>3.78</v>
       </c>
       <c r="L10" s="2">
-        <v>0.29</v>
+        <v>5.83</v>
       </c>
       <c r="M10" s="2">
-        <v>0.17</v>
+        <v>11.15</v>
       </c>
       <c r="N10" s="2">
-        <v>0.83</v>
+        <v>4.21</v>
       </c>
       <c r="O10" s="2">
-        <v>0.13</v>
+        <v>3.99</v>
       </c>
       <c r="P10" s="2">
-        <v>1.22</v>
+        <v>5.77</v>
       </c>
       <c r="Q10" s="2">
-        <v>0.96</v>
+        <v>2.34</v>
       </c>
       <c r="R10" s="2">
-        <v>1.31</v>
+        <v>2.31</v>
       </c>
       <c r="S10" s="2">
-        <v>0.7</v>
+        <v>2.01</v>
       </c>
       <c r="T10" s="2">
-        <v>0.17</v>
+        <v>2.28</v>
       </c>
       <c r="U10" s="2">
-        <v>0.1</v>
+        <v>4.82</v>
       </c>
       <c r="V10" s="2">
-        <v>0.54</v>
+        <v>40.37</v>
       </c>
       <c r="W10" s="2">
-        <v>0.66</v>
+        <v>8.01</v>
       </c>
       <c r="X10" s="2">
-        <v>0.81</v>
+        <v>2.74</v>
+      </c>
+      <c r="Y10" s="2">
+        <v>6.82</v>
+      </c>
+      <c r="Z10" s="2">
+        <v>2.85</v>
       </c>
     </row>
-    <row r="11" spans="1:24">
+    <row r="11" spans="1:26">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>0.19</v>
+        <v>1.24</v>
       </c>
       <c r="C11" s="2">
-        <v>0.08</v>
+        <v>3.91</v>
       </c>
       <c r="D11" s="2">
-        <v>0.21</v>
+        <v>2.95</v>
       </c>
       <c r="E11" s="2">
-        <v>0.13</v>
+        <v>32.16</v>
       </c>
       <c r="F11" s="2">
-        <v>0.03</v>
+        <v>2.15</v>
       </c>
       <c r="G11" s="2">
-        <v>0.08</v>
+        <v>1.84</v>
       </c>
       <c r="H11" s="2">
-        <v>0.25</v>
+        <v>3.65</v>
       </c>
       <c r="I11" s="2">
-        <v>0.23</v>
+        <v>1.55</v>
       </c>
       <c r="J11" s="2">
-        <v>0.37</v>
+        <v>1.33</v>
       </c>
       <c r="K11" s="2">
-        <v>0.15</v>
+        <v>1.85</v>
       </c>
       <c r="L11" s="2">
-        <v>0.07</v>
+        <v>2.44</v>
       </c>
       <c r="M11" s="2">
-        <v>0.04</v>
+        <v>9.64</v>
       </c>
       <c r="N11" s="2">
-        <v>0.3</v>
+        <v>3.03</v>
       </c>
       <c r="O11" s="2">
-        <v>0.02</v>
+        <v>1.53</v>
       </c>
       <c r="P11" s="2">
-        <v>0.2</v>
+        <v>1.25</v>
       </c>
       <c r="Q11" s="2">
-        <v>0.36</v>
+        <v>1.92</v>
       </c>
       <c r="R11" s="2">
-        <v>0.39</v>
+        <v>2.27</v>
       </c>
       <c r="S11" s="2">
-        <v>0.05</v>
+        <v>1.39</v>
       </c>
       <c r="T11" s="2">
-        <v>0.01</v>
+        <v>1.81</v>
       </c>
       <c r="U11" s="2">
-        <v>0.02</v>
+        <v>1.08</v>
       </c>
       <c r="V11" s="2">
-        <v>0.11</v>
+        <v>9.93</v>
       </c>
       <c r="W11" s="2">
-        <v>0.1</v>
+        <v>7.25</v>
       </c>
       <c r="X11" s="2">
-        <v>0.05</v>
+        <v>2.41</v>
+      </c>
+      <c r="Y11" s="2">
+        <v>3.29</v>
+      </c>
+      <c r="Z11" s="2">
+        <v>1.61</v>
       </c>
     </row>
-    <row r="12" spans="1:24">
+    <row r="12" spans="1:26">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="2">
-        <v>300.38</v>
+        <v>11437.33</v>
       </c>
       <c r="C12" s="2">
-        <v>822.31</v>
+        <v>7680.43</v>
       </c>
       <c r="D12" s="2">
-        <v>580.49</v>
+        <v>45530</v>
       </c>
       <c r="E12" s="2">
-        <v>15.68</v>
+        <v>123597</v>
       </c>
       <c r="F12" s="2">
-        <v>178.85</v>
+        <v>102571</v>
       </c>
       <c r="G12" s="2">
-        <v>1067.01</v>
+        <v>19510.14</v>
       </c>
       <c r="H12" s="2">
-        <v>1105.81</v>
+        <v>10187.24</v>
       </c>
       <c r="I12" s="2">
-        <v>855.2</v>
+        <v>4712.34</v>
       </c>
       <c r="J12" s="2">
-        <v>373.21</v>
+        <v>3026.46</v>
       </c>
       <c r="K12" s="2">
-        <v>1395.87</v>
+        <v>12789.81</v>
       </c>
       <c r="L12" s="2">
-        <v>1336.31</v>
+        <v>13314.77</v>
       </c>
       <c r="M12" s="2">
-        <v>277.16</v>
+        <v>8559.67</v>
       </c>
       <c r="N12" s="2">
-        <v>1579.84</v>
+        <v>6690.94</v>
       </c>
       <c r="O12" s="2">
-        <v>1072.47</v>
+        <v>118558</v>
       </c>
       <c r="P12" s="2">
-        <v>1751.63</v>
+        <v>263096</v>
       </c>
       <c r="Q12" s="2">
-        <v>635.46</v>
+        <v>68172</v>
       </c>
       <c r="R12" s="2">
-        <v>1999.28</v>
+        <v>6616.02</v>
       </c>
       <c r="S12" s="2">
-        <v>164.47</v>
+        <v>4385.59</v>
       </c>
       <c r="T12" s="2">
-        <v>-86.28</v>
+        <v>13074.4</v>
       </c>
       <c r="U12" s="2">
-        <v>390.23</v>
+        <v>4839.36</v>
       </c>
       <c r="V12" s="2">
-        <v>552.67</v>
+        <v>5041.96</v>
       </c>
       <c r="W12" s="2">
-        <v>263.36</v>
+        <v>4102.28</v>
       </c>
       <c r="X12" s="2">
-        <v>389.6</v>
+        <v>14183.04</v>
+      </c>
+      <c r="Y12" s="2">
+        <v>42483.32</v>
+      </c>
+      <c r="Z12" s="2">
+        <v>31472</v>
       </c>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13" spans="1:26">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="1">
-        <v>34.57</v>
+        <v>4.3</v>
       </c>
       <c r="C13" s="1">
-        <v>63.18</v>
+        <v>2.58</v>
       </c>
       <c r="D13" s="1">
-        <v>49.73</v>
+        <v>8.43</v>
       </c>
       <c r="E13" s="1">
-        <v>89.72</v>
+        <v>6.95</v>
       </c>
       <c r="F13" s="1">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G13" s="1">
-        <v>18.94</v>
+        <v>2.86</v>
       </c>
       <c r="H13" s="1">
-        <v>23.77</v>
+        <v>0.16</v>
       </c>
       <c r="I13" s="1">
-        <v>9.91</v>
+        <v>4.43</v>
       </c>
       <c r="J13" s="1">
-        <v>20.23</v>
+        <v>7.17</v>
       </c>
       <c r="K13" s="1">
-        <v>37.19</v>
+        <v>7.54</v>
       </c>
       <c r="L13" s="1">
-        <v>38.74</v>
+        <v>0.07</v>
       </c>
       <c r="M13" s="1">
-        <v>58.24</v>
+        <v>0.31</v>
       </c>
       <c r="N13" s="1">
-        <v>28.17</v>
+        <v>7.38</v>
       </c>
       <c r="O13" s="1">
-        <v>29.01</v>
+        <v>4.26</v>
       </c>
       <c r="P13" s="1">
-        <v>23.7</v>
+        <v>16.4</v>
       </c>
       <c r="Q13" s="1">
-        <v>17.25</v>
+        <v>6.17</v>
       </c>
       <c r="R13" s="1">
-        <v>31.92</v>
+        <v>1.19</v>
       </c>
       <c r="S13" s="1">
-        <v>61.32</v>
+        <v>1.54</v>
       </c>
       <c r="T13" s="1">
-        <v>103.07</v>
+        <v>23.53</v>
       </c>
       <c r="U13" s="1">
-        <v>65.66</v>
+        <v>7.19</v>
       </c>
       <c r="V13" s="1">
-        <v>44.4</v>
+        <v>1.83</v>
       </c>
       <c r="W13" s="1">
-        <v>20.6</v>
+        <v>1.94</v>
       </c>
       <c r="X13" s="1">
-        <v>36.82</v>
+        <v>8.39</v>
+      </c>
+      <c r="Y13" s="1">
+        <v>8.16</v>
+      </c>
+      <c r="Z13" s="1">
+        <v>13.99</v>
       </c>
     </row>
-    <row r="14" spans="1:24">
+    <row r="14" spans="1:26">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="1">
-        <v>1183.92</v>
+        <v>4.77</v>
       </c>
       <c r="C14" s="1">
-        <v>1056.9</v>
+        <v>3.06</v>
       </c>
       <c r="D14" s="1">
-        <v>123.18</v>
+        <v>10.23</v>
       </c>
       <c r="E14" s="1">
-        <v>6394.05</v>
+        <v>7.61</v>
       </c>
       <c r="F14" s="1">
-        <v>0</v>
+        <v>16.75</v>
       </c>
       <c r="G14" s="1">
-        <v>59.56</v>
+        <v>3.26</v>
       </c>
       <c r="H14" s="1">
-        <v>44.2</v>
+        <v>0.18</v>
       </c>
       <c r="I14" s="1">
-        <v>28.88</v>
+        <v>5.31</v>
       </c>
       <c r="J14" s="1">
-        <v>61.85</v>
+        <v>10.45</v>
       </c>
       <c r="K14" s="1">
-        <v>80.1</v>
+        <v>9.56</v>
       </c>
       <c r="L14" s="1">
-        <v>616.37</v>
+        <v>0.07</v>
       </c>
       <c r="M14" s="1">
-        <v>952.94</v>
+        <v>0.37</v>
       </c>
       <c r="N14" s="1">
-        <v>51.09</v>
+        <v>8.82</v>
       </c>
       <c r="O14" s="1">
-        <v>49.66</v>
+        <v>5.09</v>
       </c>
       <c r="P14" s="1">
-        <v>42.79</v>
+        <v>23.18</v>
       </c>
       <c r="Q14" s="1">
-        <v>35.85</v>
+        <v>7.13</v>
       </c>
       <c r="R14" s="1">
-        <v>66</v>
+        <v>1.23</v>
       </c>
       <c r="S14" s="1">
-        <v>1309.12</v>
+        <v>1.6</v>
       </c>
       <c r="T14" s="1">
-        <v>-410.58</v>
+        <v>34.34</v>
       </c>
       <c r="U14" s="1">
-        <v>386.53</v>
+        <v>8.99</v>
       </c>
       <c r="V14" s="1">
-        <v>149.76</v>
+        <v>2.01</v>
       </c>
       <c r="W14" s="1">
-        <v>123.47</v>
+        <v>2.13</v>
       </c>
       <c r="X14" s="1">
-        <v>76.3</v>
+        <v>10.03</v>
+      </c>
+      <c r="Y14" s="1">
+        <v>9.73</v>
+      </c>
+      <c r="Z14" s="1">
+        <v>24.06</v>
       </c>
     </row>
-    <row r="15" spans="1:24">
+    <row r="15" spans="1:26">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="2">
-        <v>16209.91</v>
+        <v>13133.84</v>
       </c>
       <c r="C15" s="2">
-        <v>16270.57</v>
+        <v>9834.97</v>
       </c>
       <c r="D15" s="2">
-        <v>1712.82</v>
+        <v>54955.5</v>
       </c>
       <c r="E15" s="2">
-        <v>630.13</v>
+        <v>135816</v>
       </c>
       <c r="F15" s="2">
-        <v>314.62</v>
+        <v>129086</v>
       </c>
       <c r="G15" s="2">
-        <v>3366.76</v>
+        <v>21423.95</v>
       </c>
       <c r="H15" s="2">
-        <v>2143.33</v>
+        <v>11243.54</v>
       </c>
       <c r="I15" s="2">
-        <v>2751.22</v>
+        <v>5870.42</v>
       </c>
       <c r="J15" s="2">
-        <v>1115.49</v>
+        <v>3504.02</v>
       </c>
       <c r="K15" s="2">
-        <v>3308.13</v>
+        <v>15353.61</v>
       </c>
       <c r="L15" s="2">
-        <v>23575.02</v>
+        <v>14186.39</v>
       </c>
       <c r="M15" s="2">
-        <v>5488.21</v>
+        <v>7990.07</v>
       </c>
       <c r="N15" s="2">
-        <v>2898.05</v>
+        <v>7540.83</v>
       </c>
       <c r="O15" s="2">
-        <v>1703.85</v>
+        <v>139366</v>
       </c>
       <c r="P15" s="2">
-        <v>3005.63</v>
+        <v>276358</v>
       </c>
       <c r="Q15" s="2">
-        <v>1566.18</v>
+        <v>78905.5</v>
       </c>
       <c r="R15" s="2">
-        <v>4370.64</v>
+        <v>6593.88</v>
       </c>
       <c r="S15" s="2">
-        <v>3702.27</v>
+        <v>4480.78</v>
       </c>
       <c r="T15" s="2">
-        <v>420.25</v>
+        <v>18513.64</v>
       </c>
       <c r="U15" s="2">
-        <v>2300</v>
+        <v>5793.91</v>
       </c>
       <c r="V15" s="2">
-        <v>1958.95</v>
+        <v>5040.54</v>
       </c>
       <c r="W15" s="2">
-        <v>1671.56</v>
+        <v>4292.75</v>
       </c>
       <c r="X15" s="2">
-        <v>634.61</v>
+        <v>17104.8</v>
+      </c>
+      <c r="Y15" s="2">
+        <v>40377.25</v>
+      </c>
+      <c r="Z15" s="2">
+        <v>50862.5</v>
       </c>
     </row>
-    <row r="16" spans="1:24">
+    <row r="16" spans="1:26">
       <c r="A16" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="2">
-        <v>3189.66</v>
+        <v>11944.58</v>
       </c>
       <c r="C16" s="2">
-        <v>3176.4</v>
+        <v>8270.26</v>
       </c>
       <c r="D16" s="2">
-        <v>701.87</v>
+        <v>47848.5</v>
       </c>
       <c r="E16" s="2">
-        <v>43.58</v>
+        <v>123342.5</v>
       </c>
       <c r="F16" s="2">
-        <v>182.65</v>
+        <v>106152.5</v>
       </c>
       <c r="G16" s="2">
-        <v>1272.21</v>
+        <v>19229.91</v>
       </c>
       <c r="H16" s="2">
-        <v>1211.72</v>
+        <v>9967.13</v>
       </c>
       <c r="I16" s="2">
-        <v>1556.84</v>
+        <v>4581.34</v>
       </c>
       <c r="J16" s="2">
-        <v>393.58</v>
+        <v>3310.41</v>
       </c>
       <c r="K16" s="2">
-        <v>1628.88</v>
+        <v>12399.85</v>
       </c>
       <c r="L16" s="2">
-        <v>2231.67</v>
+        <v>12358.65</v>
       </c>
       <c r="M16" s="2">
-        <v>979.21</v>
+        <v>7108.14</v>
       </c>
       <c r="N16" s="2">
-        <v>1686.93</v>
+        <v>6138.41</v>
       </c>
       <c r="O16" s="2">
-        <v>890.95</v>
+        <v>115987.5</v>
       </c>
       <c r="P16" s="2">
-        <v>2010.25</v>
+        <v>193439.5</v>
       </c>
       <c r="Q16" s="2">
-        <v>922.17</v>
+        <v>70748.5</v>
       </c>
       <c r="R16" s="2">
-        <v>2430.36</v>
+        <v>6327.29</v>
       </c>
       <c r="S16" s="2">
-        <v>203.33</v>
+        <v>4324.45</v>
       </c>
       <c r="T16" s="2">
-        <v>2.65</v>
+        <v>13071.56</v>
       </c>
       <c r="U16" s="2">
-        <v>671.47</v>
+        <v>4352.28</v>
       </c>
       <c r="V16" s="2">
-        <v>711.42</v>
+        <v>4730.41</v>
       </c>
       <c r="W16" s="2">
-        <v>407.92</v>
+        <v>3757.47</v>
       </c>
       <c r="X16" s="2">
-        <v>347.11</v>
+        <v>13811.17</v>
+      </c>
+      <c r="Y16" s="2">
+        <v>34002.22</v>
+      </c>
+      <c r="Z16" s="2">
+        <v>36465.5</v>
       </c>
     </row>
-    <row r="17" spans="1:24">
+    <row r="17" spans="1:26">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="1">
-        <v>-22.78</v>
+        <v>7.34</v>
       </c>
       <c r="C17" s="1">
-        <v>-20.72</v>
+        <v>13.54</v>
       </c>
       <c r="D17" s="1">
-        <v>-25.51</v>
+        <v>5.16</v>
       </c>
       <c r="E17" s="1">
-        <v>-19.83</v>
+        <v>5.69</v>
       </c>
       <c r="F17" s="1">
-        <v>-11.15</v>
+        <v>8.65</v>
       </c>
       <c r="G17" s="1">
-        <v>-7</v>
+        <v>10.89</v>
       </c>
       <c r="H17" s="1">
-        <v>-4.55</v>
+        <v>12.9</v>
       </c>
       <c r="I17" s="1">
-        <v>-9.06</v>
+        <v>22.61</v>
       </c>
       <c r="J17" s="1">
-        <v>-10.03</v>
+        <v>10.19</v>
       </c>
       <c r="K17" s="1">
-        <v>-11.4</v>
+        <v>8.7</v>
       </c>
       <c r="L17" s="1">
-        <v>-14.21</v>
+        <v>17.45</v>
       </c>
       <c r="M17" s="1">
-        <v>-26.74</v>
+        <v>8.12</v>
       </c>
       <c r="N17" s="1">
-        <v>-6.23</v>
+        <v>6.38</v>
       </c>
       <c r="O17" s="1">
-        <v>-8.74</v>
+        <v>6.72</v>
       </c>
       <c r="P17" s="1">
-        <v>-14.08</v>
+        <v>6.19</v>
       </c>
       <c r="Q17" s="1">
-        <v>-17.16</v>
+        <v>3.68</v>
       </c>
       <c r="R17" s="1">
-        <v>-8.3</v>
+        <v>8.1</v>
       </c>
       <c r="S17" s="1">
-        <v>-3.11</v>
+        <v>3.85</v>
       </c>
       <c r="T17" s="1">
-        <v>-42.95</v>
+        <v>7.76</v>
       </c>
       <c r="U17" s="1">
-        <v>-8.04</v>
+        <v>8</v>
       </c>
       <c r="V17" s="1">
-        <v>-18.23</v>
+        <v>14.15</v>
       </c>
       <c r="W17" s="1">
-        <v>-11.51</v>
+        <v>8.61</v>
       </c>
       <c r="X17" s="1">
-        <v>-14.13</v>
+        <v>7.92</v>
+      </c>
+      <c r="Y17" s="1">
+        <v>40.71</v>
+      </c>
+      <c r="Z17" s="1">
+        <v>7.68</v>
       </c>
     </row>
-    <row r="18" spans="1:24">
+    <row r="18" spans="1:26">
       <c r="A18" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="2">
-        <v>5.08</v>
+        <v>1.1</v>
       </c>
       <c r="C18" s="2">
-        <v>5.12</v>
+        <v>1.19</v>
       </c>
       <c r="D18" s="2">
-        <v>2.44</v>
+        <v>1.15</v>
       </c>
       <c r="E18" s="2">
-        <v>14.46</v>
+        <v>1.1</v>
       </c>
       <c r="F18" s="2">
-        <v>1.72</v>
+        <v>1.22</v>
       </c>
       <c r="G18" s="2">
-        <v>2.65</v>
+        <v>1.11</v>
       </c>
       <c r="H18" s="2">
-        <v>1.77</v>
+        <v>1.13</v>
       </c>
       <c r="I18" s="2">
-        <v>1.77</v>
+        <v>1.28</v>
       </c>
       <c r="J18" s="2">
-        <v>2.83</v>
+        <v>1.06</v>
       </c>
       <c r="K18" s="2">
-        <v>2.03</v>
+        <v>1.24</v>
       </c>
       <c r="L18" s="2">
-        <v>10.56</v>
+        <v>1.15</v>
       </c>
       <c r="M18" s="2">
-        <v>5.6</v>
+        <v>1.12</v>
       </c>
       <c r="N18" s="2">
-        <v>1.72</v>
+        <v>1.23</v>
       </c>
       <c r="O18" s="2">
-        <v>1.91</v>
+        <v>1.2</v>
       </c>
       <c r="P18" s="2">
-        <v>1.5</v>
+        <v>1.43</v>
       </c>
       <c r="Q18" s="2">
-        <v>1.7</v>
+        <v>1.12</v>
       </c>
       <c r="R18" s="2">
-        <v>1.8</v>
+        <v>1.04</v>
       </c>
       <c r="S18" s="2">
-        <v>18.21</v>
+        <v>1.04</v>
       </c>
       <c r="T18" s="2">
-        <v>158.55</v>
+        <v>1.42</v>
       </c>
       <c r="U18" s="2">
-        <v>3.43</v>
+        <v>1.33</v>
       </c>
       <c r="V18" s="2">
-        <v>2.75</v>
+        <v>1.07</v>
       </c>
       <c r="W18" s="2">
-        <v>4.1</v>
+        <v>1.14</v>
       </c>
       <c r="X18" s="2">
-        <v>1.83</v>
+        <v>1.24</v>
+      </c>
+      <c r="Y18" s="2">
+        <v>1.19</v>
+      </c>
+      <c r="Z18" s="2">
+        <v>1.39</v>
       </c>
     </row>
-    <row r="19" spans="1:24">
+    <row r="19" spans="1:26">
       <c r="A19" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="1">
-        <v>6.13</v>
+        <v>5.57</v>
       </c>
       <c r="C19" s="1">
-        <v>38.72</v>
+        <v>4.27</v>
       </c>
       <c r="D19" s="1">
-        <v>50.06</v>
+        <v>11.16</v>
       </c>
       <c r="E19" s="1">
-        <v>187.01</v>
+        <v>7.21</v>
       </c>
       <c r="F19" s="1">
-        <v>0.68</v>
+        <v>16.69</v>
       </c>
       <c r="G19" s="1">
-        <v>3.54</v>
+        <v>4.89</v>
       </c>
       <c r="H19" s="1">
-        <v>0.24</v>
+        <v>7.34</v>
       </c>
       <c r="I19" s="1">
-        <v>4.23</v>
+        <v>6.55</v>
       </c>
       <c r="J19" s="1">
-        <v>3.01</v>
+        <v>4.09</v>
       </c>
       <c r="K19" s="1">
-        <v>3.13</v>
+        <v>3.09</v>
       </c>
       <c r="L19" s="1">
-        <v>41.4</v>
+        <v>18.52</v>
       </c>
       <c r="M19" s="1">
-        <v>2639.57</v>
+        <v>5.75</v>
       </c>
       <c r="N19" s="1">
-        <v>0.07</v>
+        <v>3.37</v>
       </c>
       <c r="O19" s="1">
-        <v>42.56</v>
+        <v>3.62</v>
       </c>
       <c r="P19" s="1">
-        <v>8.78</v>
+        <v>3.93</v>
       </c>
       <c r="Q19" s="1">
-        <v>3.91</v>
+        <v>3.88</v>
       </c>
       <c r="R19" s="1">
-        <v>1.15</v>
+        <v>11.81</v>
       </c>
       <c r="S19" s="1">
-        <v>12.57</v>
+        <v>3.15</v>
       </c>
       <c r="T19" s="1">
-        <v>16031.53</v>
+        <v>19.58</v>
       </c>
       <c r="U19" s="1">
-        <v>55.5</v>
+        <v>10.14</v>
       </c>
       <c r="V19" s="1">
-        <v>23.63</v>
+        <v>124.56</v>
       </c>
       <c r="W19" s="1">
-        <v>5.2</v>
+        <v>7.26</v>
       </c>
       <c r="X19" s="1">
-        <v>5.43</v>
+        <v>4.85</v>
+      </c>
+      <c r="Y19" s="1">
+        <v>154.03</v>
+      </c>
+      <c r="Z19" s="1">
+        <v>7.21</v>
       </c>
     </row>
-    <row r="20" spans="1:24">
+    <row r="20" spans="1:26">
       <c r="A20" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="2">
-        <v>1.31</v>
+        <v>10.54</v>
       </c>
       <c r="C20" s="2">
-        <v>0.77</v>
+        <v>29.06</v>
       </c>
       <c r="D20" s="2">
-        <v>1.48</v>
+        <v>2.83</v>
       </c>
       <c r="E20" s="2">
-        <v>1.28</v>
+        <v>10.09</v>
       </c>
       <c r="F20" s="2">
-        <v>-0.05</v>
+        <v>6.72</v>
       </c>
       <c r="G20" s="2">
-        <v>1.24</v>
+        <v>28.66</v>
       </c>
       <c r="H20" s="2">
-        <v>0.94</v>
+        <v>307.3</v>
       </c>
       <c r="I20" s="2">
-        <v>1.91</v>
+        <v>55.38</v>
       </c>
       <c r="J20" s="2">
-        <v>1.71</v>
+        <v>8.98</v>
       </c>
       <c r="K20" s="2">
-        <v>1.04</v>
+        <v>5.27</v>
       </c>
       <c r="L20" s="2">
-        <v>0.19</v>
+        <v>1200.01</v>
       </c>
       <c r="M20" s="2">
-        <v>0.3</v>
+        <v>94.76</v>
       </c>
       <c r="N20" s="2">
-        <v>1.65</v>
+        <v>2.04</v>
       </c>
       <c r="O20" s="2">
-        <v>0.84</v>
+        <v>8.02</v>
       </c>
       <c r="P20" s="2">
-        <v>1.54</v>
+        <v>2.66</v>
       </c>
       <c r="Q20" s="2">
-        <v>1.57</v>
+        <v>4.18</v>
       </c>
       <c r="R20" s="2">
-        <v>1.43</v>
+        <v>18.7</v>
       </c>
       <c r="S20" s="2">
-        <v>0.13</v>
+        <v>11.14</v>
       </c>
       <c r="T20" s="2">
-        <v>0.82</v>
+        <v>2.2</v>
       </c>
       <c r="U20" s="2">
-        <v>0.49</v>
+        <v>2.95</v>
       </c>
       <c r="V20" s="2">
-        <v>1.82</v>
+        <v>11.55</v>
       </c>
       <c r="W20" s="2">
-        <v>0.79</v>
+        <v>8.67</v>
       </c>
       <c r="X20" s="2">
-        <v>1.26</v>
+        <v>3.27</v>
+      </c>
+      <c r="Y20" s="2">
+        <v>21.31</v>
+      </c>
+      <c r="Z20" s="2">
+        <v>6.04</v>
       </c>
     </row>
-    <row r="21" spans="1:24">
+    <row r="21" spans="1:26">
       <c r="A21" t="s">
         <v>20</v>
       </c>
       <c r="B21" s="2">
-        <v>-0.06</v>
+        <v>9.26</v>
       </c>
       <c r="C21" s="2">
-        <v>-0.33</v>
+        <v>8.12</v>
       </c>
       <c r="D21" s="2">
-        <v>-1.42</v>
+        <v>7.37</v>
       </c>
       <c r="E21" s="2">
-        <v>-1.37</v>
+        <v>19.05</v>
       </c>
       <c r="F21" s="2">
-        <v>-1.62</v>
+        <v>16.77</v>
       </c>
       <c r="G21" s="2">
-        <v>-2.91</v>
+        <v>12.98</v>
       </c>
       <c r="H21" s="2">
-        <v>-4.29</v>
+        <v>6.35</v>
       </c>
       <c r="I21" s="2">
-        <v>-1.81</v>
+        <v>16.87</v>
       </c>
       <c r="J21" s="2">
-        <v>-2.34</v>
+        <v>12.06</v>
       </c>
       <c r="K21" s="2">
-        <v>-0.97</v>
+        <v>6.71</v>
       </c>
       <c r="L21" s="2">
-        <v>-0.54</v>
+        <v>8.03</v>
       </c>
       <c r="M21" s="2">
-        <v>-0.55</v>
+        <v>7.52</v>
       </c>
       <c r="N21" s="2">
-        <v>-7.95</v>
+        <v>2.76</v>
       </c>
       <c r="O21" s="2">
-        <v>-4.68</v>
+        <v>8.17</v>
       </c>
       <c r="P21" s="2">
-        <v>-2.15</v>
+        <v>10.48</v>
       </c>
       <c r="Q21" s="2">
-        <v>-1.28</v>
+        <v>11.48</v>
       </c>
       <c r="R21" s="2">
-        <v>-2.81</v>
+        <v>4.81</v>
       </c>
       <c r="S21" s="2">
-        <v>-6.4</v>
+        <v>7.55</v>
       </c>
       <c r="T21" s="2">
-        <v>-0.57</v>
+        <v>8.99</v>
       </c>
       <c r="U21" s="2">
-        <v>-7.12</v>
+        <v>3.18</v>
       </c>
       <c r="V21" s="2">
-        <v>-5.14</v>
+        <v>2.6</v>
       </c>
       <c r="W21" s="2">
-        <v>-0.84</v>
+        <v>3.19</v>
       </c>
       <c r="X21" s="2">
-        <v>-3.03</v>
+        <v>5.46</v>
+      </c>
+      <c r="Y21" s="2">
+        <v>9.13</v>
+      </c>
+      <c r="Z21" s="2">
+        <v>18.05</v>
       </c>
     </row>
-    <row r="22" spans="1:24">
+    <row r="22" spans="1:26">
       <c r="A22" t="s">
         <v>21</v>
       </c>
       <c r="B22" s="2">
-        <v>0.06</v>
+        <v>1.34</v>
       </c>
       <c r="C22" s="2">
-        <v>0.18</v>
+        <v>24.67</v>
       </c>
       <c r="D22" s="2">
-        <v>0.64</v>
+        <v>24.01</v>
       </c>
       <c r="E22" s="2">
-        <v>0.14</v>
+        <v>69.02</v>
       </c>
       <c r="F22" s="2">
-        <v>0.02</v>
+        <v>70.64</v>
       </c>
       <c r="G22" s="2">
-        <v>4.06</v>
+        <v>13.99</v>
       </c>
       <c r="H22" s="2">
-        <v>0.24</v>
+        <v>2.96</v>
       </c>
       <c r="I22" s="2">
-        <v>3.76</v>
+        <v>5.81</v>
       </c>
       <c r="J22" s="2">
-        <v>0.49</v>
+        <v>0.28</v>
       </c>
       <c r="K22" s="2">
-        <v>0.19</v>
+        <v>3.96</v>
       </c>
       <c r="L22" s="2">
-        <v>0.2</v>
+        <v>1.65</v>
       </c>
       <c r="M22" s="2">
-        <v>0.24</v>
+        <v>0.66</v>
       </c>
       <c r="N22" s="2">
-        <v>0.52</v>
+        <v>0.7</v>
       </c>
       <c r="O22" s="2">
-        <v>0.21</v>
+        <v>12.43</v>
       </c>
       <c r="P22" s="2">
-        <v>0.68</v>
+        <v>46.65</v>
       </c>
       <c r="Q22" s="2">
-        <v>0.31</v>
+        <v>31.86</v>
       </c>
       <c r="R22" s="2">
-        <v>0.31</v>
+        <v>3.21</v>
       </c>
       <c r="S22" s="2">
-        <v>0.19</v>
+        <v>11.82</v>
       </c>
       <c r="T22" s="2">
-        <v>0.19</v>
+        <v>18.98</v>
       </c>
       <c r="U22" s="2">
-        <v>0.09</v>
+        <v>0.22</v>
       </c>
       <c r="V22" s="2">
-        <v>0.22</v>
+        <v>0.26</v>
       </c>
       <c r="W22" s="2">
-        <v>0.32</v>
+        <v>0.39</v>
       </c>
       <c r="X22" s="2">
-        <v>0.06</v>
+        <v>12.81</v>
+      </c>
+      <c r="Y22" s="2">
+        <v>2.27</v>
+      </c>
+      <c r="Z22" s="2">
+        <v>11.25</v>
       </c>
     </row>
-    <row r="23" spans="1:24">
+    <row r="23" spans="1:26">
       <c r="A23" t="s">
         <v>22</v>
       </c>
       <c r="B23" s="2">
-        <v>0.08</v>
+        <v>1.69</v>
       </c>
       <c r="C23" s="2">
-        <v>0.18</v>
+        <v>26.75</v>
       </c>
       <c r="D23" s="2">
-        <v>0.73</v>
+        <v>27.25</v>
       </c>
       <c r="E23" s="2">
-        <v>0.1</v>
+        <v>77.4</v>
       </c>
       <c r="F23" s="2">
-        <v>0.02</v>
+        <v>69.25</v>
       </c>
       <c r="G23" s="2">
-        <v>3.06</v>
+        <v>15.24</v>
       </c>
       <c r="H23" s="2">
+        <v>2.88</v>
+      </c>
+      <c r="I23" s="2">
+        <v>5.77</v>
+      </c>
+      <c r="J23" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="K23" s="2">
+        <v>4.78</v>
+      </c>
+      <c r="L23" s="2">
+        <v>1.75</v>
+      </c>
+      <c r="M23" s="2">
+        <v>0.47</v>
+      </c>
+      <c r="N23" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="O23" s="2">
+        <v>13.62</v>
+      </c>
+      <c r="P23" s="2">
+        <v>54.8</v>
+      </c>
+      <c r="Q23" s="2">
+        <v>37.5</v>
+      </c>
+      <c r="R23" s="2">
+        <v>3.9</v>
+      </c>
+      <c r="S23" s="2">
+        <v>12.76</v>
+      </c>
+      <c r="T23" s="2">
+        <v>19.08</v>
+      </c>
+      <c r="U23" s="2">
+        <v>0.28</v>
+      </c>
+      <c r="V23" s="2">
         <v>0.33</v>
       </c>
-      <c r="I23" s="2">
-        <v>3.2</v>
-      </c>
-      <c r="J23" s="2">
-        <v>0.41</v>
-      </c>
-      <c r="K23" s="2">
-        <v>0.22</v>
-      </c>
-      <c r="L23" s="2">
-        <v>0.24</v>
-      </c>
-      <c r="M23" s="2">
-        <v>0.24</v>
-      </c>
-      <c r="N23" s="2">
-        <v>0.51</v>
-      </c>
-      <c r="O23" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="P23" s="2">
-        <v>0.57</v>
-      </c>
-      <c r="Q23" s="2">
-        <v>0.33</v>
-      </c>
-      <c r="R23" s="2">
-        <v>0.41</v>
-      </c>
-      <c r="S23" s="2">
-        <v>0.16</v>
-      </c>
-      <c r="T23" s="2">
-        <v>0.17</v>
-      </c>
-      <c r="U23" s="2">
-        <v>0.07</v>
-      </c>
-      <c r="V23" s="2">
-        <v>0.22</v>
-      </c>
       <c r="W23" s="2">
-        <v>0.4</v>
+        <v>0.39</v>
       </c>
       <c r="X23" s="2">
-        <v>0.06</v>
+        <v>13.68</v>
+      </c>
+      <c r="Y23" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="Z23" s="2">
+        <v>11.62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>